<commit_message>
Reflect recent extension of wind PTC in fuels/BS; change source for solar capital costs to NREL ATB in elec/CCaMC.
</commit_message>
<xml_diff>
--- a/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
+++ b/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="243">
   <si>
     <t>Onshore Wind</t>
   </si>
@@ -613,12 +613,6 @@
     <t>Gas-CT-AvgCF - Low</t>
   </si>
   <si>
-    <t>Solar Energy Industries Association</t>
-  </si>
-  <si>
-    <t>"National Solar PV System Pricing" section, last paragraph (using "fixed-tilt" value)</t>
-  </si>
-  <si>
     <t>curves to determine cost declines.  Therefore, we only specify the first simulated year costs in this spreadsheet,</t>
   </si>
   <si>
@@ -712,12 +706,6 @@
     <t>We adjust 2018 dollars to 2012 dollars using the following conversion factor:</t>
   </si>
   <si>
-    <t>U.S. Solar Market Insight Report: 2018 Year in Review (Executive Summary)</t>
-  </si>
-  <si>
-    <t>https://www.seia.org/research-resources/solar-market-insight-report-2018-year-review</t>
-  </si>
-  <si>
     <t>crude oil</t>
   </si>
   <si>
@@ -745,9 +733,6 @@
     <t>so we use the cost improvement rates for biomass power plants.</t>
   </si>
   <si>
-    <t>2018 Solar Capital Cost</t>
-  </si>
-  <si>
     <t>AEO 2019</t>
   </si>
   <si>
@@ -841,7 +826,7 @@
     <t>2018 Onshore Wind Capital Cost</t>
   </si>
   <si>
-    <t>Cost Improvement Rate and Offshore Wind Costs</t>
+    <t>2018 Solar Capital Cost, Cost Imrpovement Rates, and Offshore Wind Costs</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1588,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1761,6 +1746,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="228">
@@ -2351,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2387,11 +2375,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="15" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E5" s="8"/>
     </row>
@@ -2405,7 +2393,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D7" s="2">
         <v>2018</v>
@@ -2413,10 +2401,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2424,15 +2412,15 @@
         <v>55</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2444,15 +2432,15 @@
         <v>124</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>171</v>
+      <c r="D13" s="53" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2467,8 +2455,8 @@
       <c r="B15" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>204</v>
+      <c r="D15" s="53" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2476,16 +2464,14 @@
         <v>127</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="B17" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>172</v>
-      </c>
+      <c r="D17" s="19"/>
     </row>
     <row r="18" spans="1:11">
       <c r="B18" s="23"/>
@@ -2495,45 +2481,34 @@
       <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>247</v>
-      </c>
+      <c r="D19" s="64"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>146</v>
-      </c>
+      <c r="D20" s="23"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7"/>
       <c r="B21" s="2">
         <v>2015</v>
       </c>
-      <c r="D21" s="2">
-        <v>2019</v>
-      </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>236</v>
-      </c>
+      <c r="D22" s="23"/>
     </row>
     <row r="23" spans="1:11" ht="45">
       <c r="A23" s="7"/>
       <c r="B23" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>242</v>
-      </c>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1">
       <c r="A24" s="7"/>
@@ -2587,7 +2562,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="10" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="11"/>
@@ -2600,7 +2575,7 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="10" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="11"/>
@@ -2637,7 +2612,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="11"/>
@@ -2676,7 +2651,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="10" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="11"/>
@@ -2876,7 +2851,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="11"/>
@@ -2889,7 +2864,7 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="11"/>
@@ -2940,7 +2915,7 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="10" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B58" s="9"/>
       <c r="D58" s="7"/>
@@ -2954,7 +2929,7 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="10" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B59" s="9"/>
       <c r="D59" s="7"/>
@@ -2996,7 +2971,7 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B62" s="9"/>
       <c r="D62" s="7"/>
@@ -3280,13 +3255,12 @@
   <hyperlinks>
     <hyperlink ref="B23" r:id="rId1" display="http://rredc.nrel.gov/solar/calculators/pvwatts/system.html"/>
     <hyperlink ref="B16" r:id="rId2"/>
-    <hyperlink ref="D16" r:id="rId3"/>
-    <hyperlink ref="B9" r:id="rId4"/>
-    <hyperlink ref="D9" r:id="rId5"/>
-    <hyperlink ref="D23" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="D16" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -3328,10 +3302,10 @@
         <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3354,7 +3328,7 @@
         <v>31.16</v>
       </c>
       <c r="G2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H2">
         <v>2013</v>
@@ -3368,7 +3342,7 @@
         <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3">
         <v>5169</v>
@@ -3380,7 +3354,7 @@
         <v>72.12</v>
       </c>
       <c r="G3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H3">
         <v>2018</v>
@@ -3406,7 +3380,7 @@
         <v>11.33</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H4" s="53">
         <v>2018</v>
@@ -3432,7 +3406,7 @@
         <v>10.3</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H5" s="53">
         <v>2018</v>
@@ -3458,7 +3432,7 @@
         <v>18.03</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H6" s="53">
         <v>2018</v>
@@ -3484,7 +3458,7 @@
         <v>7.01</v>
       </c>
       <c r="G7" s="53" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H7" s="53">
         <v>2018</v>
@@ -3510,7 +3484,7 @@
         <v>103.31</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H8" s="53">
         <v>2018</v>
@@ -3536,7 +3510,7 @@
         <v>114.39</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H9" s="53">
         <v>2018</v>
@@ -3562,7 +3536,7 @@
         <v>122.28</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H10" s="53">
         <v>2018</v>
@@ -3588,7 +3562,7 @@
         <v>40.85</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H11" s="53">
         <v>2018</v>
@@ -3614,7 +3588,7 @@
         <v>48.42</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H12" s="53">
         <v>2018</v>
@@ -3640,7 +3614,7 @@
         <v>80.14</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H13" s="53">
         <v>2018</v>
@@ -3666,7 +3640,7 @@
         <v>72.84</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H14" s="53">
         <v>2018</v>
@@ -3692,7 +3666,7 @@
         <v>22.46</v>
       </c>
       <c r="G15" s="53" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H15" s="53">
         <v>2018</v>
@@ -3700,13 +3674,13 @@
     </row>
     <row r="16" spans="1:8" s="23" customFormat="1">
       <c r="A16" s="23" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D16" s="52">
         <v>8895</v>
@@ -3718,7 +3692,7 @@
         <v>425.38</v>
       </c>
       <c r="G16" s="53" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H16" s="53">
         <v>2018</v>
@@ -3744,7 +3718,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3755,7 +3729,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="19" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
@@ -3777,7 +3751,7 @@
     <row r="4" spans="1:2" s="19" customFormat="1"/>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="19" customFormat="1">
@@ -3793,7 +3767,7 @@
         <v>2018</v>
       </c>
       <c r="B7" s="16">
-        <v>1.04</v>
+        <v>1.0960000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4596,7 +4570,7 @@
   <sheetData>
     <row r="1" spans="1:36" s="23" customFormat="1">
       <c r="A1" s="55" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -4749,7 +4723,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C3" s="53">
         <v>5179.5016296472777</v>
@@ -4859,7 +4833,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4" s="53">
         <v>906.43752501948961</v>
@@ -8489,7 +8463,7 @@
         <v>120</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C37" s="53">
         <v>4654.7690040318539</v>
@@ -8599,7 +8573,7 @@
         <v>120</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C38" s="53">
         <v>4598.9063450796984</v>
@@ -8709,7 +8683,7 @@
         <v>120</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C39" s="53">
         <v>4826.7338115915436</v>
@@ -8819,7 +8793,7 @@
         <v>120</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C40" s="53">
         <v>4996.613495139718</v>
@@ -8929,7 +8903,7 @@
         <v>120</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C41" s="53">
         <v>5256.8000129437169</v>
@@ -9037,7 +9011,7 @@
     <row r="42" spans="1:36" s="23" customFormat="1"/>
     <row r="43" spans="1:36" s="53" customFormat="1">
       <c r="A43" s="55" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B43" s="55"/>
     </row>
@@ -9047,7 +9021,7 @@
     </row>
     <row r="45" spans="1:36" s="53" customFormat="1">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B45" s="23">
         <v>12.491269722013936</v>
@@ -9055,7 +9029,7 @@
     </row>
     <row r="46" spans="1:36" s="53" customFormat="1">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B46" s="23">
         <v>24.982539444027871</v>
@@ -9063,7 +9037,7 @@
     </row>
     <row r="47" spans="1:36" s="53" customFormat="1">
       <c r="A47" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B47" s="23">
         <v>49.965078888055743</v>
@@ -9071,7 +9045,7 @@
     </row>
     <row r="48" spans="1:36" s="53" customFormat="1">
       <c r="A48" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B48" s="23">
         <v>320</v>
@@ -9079,7 +9053,7 @@
     </row>
     <row r="49" spans="1:35" s="53" customFormat="1">
       <c r="A49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B49" s="23">
         <v>320</v>
@@ -9087,7 +9061,7 @@
     </row>
     <row r="50" spans="1:35" s="53" customFormat="1">
       <c r="A50" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B50" s="23">
         <v>12.491269722013936</v>
@@ -9095,7 +9069,7 @@
     </row>
     <row r="51" spans="1:35" s="53" customFormat="1">
       <c r="A51" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B51" s="23">
         <v>24.982539444027871</v>
@@ -9103,7 +9077,7 @@
     </row>
     <row r="52" spans="1:35" s="53" customFormat="1">
       <c r="A52" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B52" s="23">
         <v>49.965078888055743</v>
@@ -9111,7 +9085,7 @@
     </row>
     <row r="53" spans="1:35" s="53" customFormat="1">
       <c r="A53" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B53" s="23">
         <v>99.930157776111486</v>
@@ -9119,7 +9093,7 @@
     </row>
     <row r="54" spans="1:35" s="53" customFormat="1">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B54" s="23">
         <v>199.86031555222297</v>
@@ -9127,7 +9101,7 @@
     </row>
     <row r="55" spans="1:35" s="53" customFormat="1">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B55" s="23">
         <v>199.86031555222297</v>
@@ -9135,7 +9109,7 @@
     </row>
     <row r="56" spans="1:35" s="53" customFormat="1">
       <c r="A56" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B56" s="23">
         <v>199.86031555222297</v>
@@ -9143,7 +9117,7 @@
     </row>
     <row r="57" spans="1:35" s="53" customFormat="1">
       <c r="A57" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B57" s="23">
         <v>199.86031555222297</v>
@@ -9151,7 +9125,7 @@
     </row>
     <row r="58" spans="1:35" s="53" customFormat="1">
       <c r="A58" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B58" s="23">
         <v>199.86031555222297</v>
@@ -9159,7 +9133,7 @@
     </row>
     <row r="59" spans="1:35" s="53" customFormat="1">
       <c r="A59" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B59" s="23">
         <v>143.39977640871999</v>
@@ -9168,7 +9142,7 @@
     <row r="60" spans="1:35" s="53" customFormat="1"/>
     <row r="61" spans="1:35" s="23" customFormat="1">
       <c r="A61" s="55" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B61" s="54"/>
       <c r="C61" s="54"/>
@@ -10443,139 +10417,139 @@
         <v>120</v>
       </c>
       <c r="B71" s="23">
-        <f>(SUMPRODUCT(C$27:C$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" ref="B71:AI71" si="8">(SUMPRODUCT(C$27:C$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
         <v>1</v>
       </c>
       <c r="C71" s="23">
-        <f>(SUMPRODUCT(D$27:D$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.76893251532958939</v>
       </c>
       <c r="D71" s="23">
-        <f>(SUMPRODUCT(E$27:E$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.73908611988359929</v>
       </c>
       <c r="E71" s="23">
-        <f>(SUMPRODUCT(F$27:F$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.71041231821700446</v>
       </c>
       <c r="F71" s="23">
-        <f>(SUMPRODUCT(G$27:G$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.68286455787608569</v>
       </c>
       <c r="G71" s="23">
-        <f>(SUMPRODUCT(H$27:H$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.65639815098108378</v>
       </c>
       <c r="H71" s="23">
-        <f>(SUMPRODUCT(I$27:I$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.63097019899268714</v>
       </c>
       <c r="I71" s="23">
-        <f>(SUMPRODUCT(J$27:J$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.60653952053245963</v>
       </c>
       <c r="J71" s="23">
-        <f>(SUMPRODUCT(K$27:K$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.58306658213263374</v>
       </c>
       <c r="K71" s="23">
-        <f>(SUMPRODUCT(L$27:L$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.56051343179579671</v>
       </c>
       <c r="L71" s="23">
-        <f>(SUMPRODUCT(M$27:M$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.53884363524988776</v>
       </c>
       <c r="M71" s="23">
-        <f>(SUMPRODUCT(N$27:N$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.51802221478861732</v>
       </c>
       <c r="N71" s="23">
-        <f>(SUMPRODUCT(O$27:O$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.49801559059191758</v>
       </c>
       <c r="O71" s="23">
-        <f>(SUMPRODUCT(P$27:P$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.47879152442534423</v>
       </c>
       <c r="P71" s="23">
-        <f>(SUMPRODUCT(Q$27:Q$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.46031906562148955</v>
       </c>
       <c r="Q71" s="23">
-        <f>(SUMPRODUCT(R$27:R$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.44256849925043112</v>
       </c>
       <c r="R71" s="23">
-        <f>(SUMPRODUCT(S$27:S$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.4255112963900457</v>
       </c>
       <c r="S71" s="23">
-        <f>(SUMPRODUCT(T$27:T$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.40912006641066312</v>
       </c>
       <c r="T71" s="23">
-        <f>(SUMPRODUCT(U$27:U$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.39336851119203725</v>
       </c>
       <c r="U71" s="23">
-        <f>(SUMPRODUCT(V$27:V$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.3782313811939606</v>
       </c>
       <c r="V71" s="23">
-        <f>(SUMPRODUCT(W$27:W$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.36368443330506955</v>
       </c>
       <c r="W71" s="23">
-        <f>(SUMPRODUCT(X$27:X$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.34970439039746898</v>
       </c>
       <c r="X71" s="23">
-        <f>(SUMPRODUCT(Y$27:Y$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.33626890251776775</v>
       </c>
       <c r="Y71" s="23">
-        <f>(SUMPRODUCT(Z$27:Z$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.3233565096479471</v>
       </c>
       <c r="Z71" s="23">
-        <f>(SUMPRODUCT(AA$27:AA$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.31094660597221052</v>
       </c>
       <c r="AA71" s="23">
-        <f>(SUMPRODUCT(AB$27:AB$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.29901940558856843</v>
       </c>
       <c r="AB71" s="23">
-        <f>(SUMPRODUCT(AC$27:AC$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.2875559096064163</v>
       </c>
       <c r="AC71" s="23">
-        <f>(SUMPRODUCT(AD$27:AD$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.27653787457376039</v>
       </c>
       <c r="AD71" s="23">
-        <f>(SUMPRODUCT(AE$27:AE$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.26594778218005038</v>
       </c>
       <c r="AE71" s="23">
-        <f>(SUMPRODUCT(AF$27:AF$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.25576881018278191</v>
       </c>
       <c r="AF71" s="23">
-        <f>(SUMPRODUCT(AG$27:AG$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.24598480450814955</v>
       </c>
       <c r="AG71" s="23">
-        <f>(SUMPRODUCT(AH$27:AH$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.23658025247806094</v>
       </c>
       <c r="AH71" s="23">
-        <f>(SUMPRODUCT(AI$27:AI$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.22754025711776654</v>
       </c>
       <c r="AI71" s="23">
-        <f>(SUMPRODUCT(AJ$27:AJ$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
+        <f t="shared" si="8"/>
         <v>0.21885051250023072</v>
       </c>
     </row>
@@ -10828,7 +10802,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B15" s="4">
         <f>B11</f>
@@ -10844,7 +10818,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B16" s="4">
         <f>B11</f>
@@ -10860,7 +10834,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B17" s="4">
         <f>('EIA Costs'!F16*1000)*(About!$A$63)</f>
@@ -11123,7 +11097,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="23" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B15" s="16">
         <f>B11</f>
@@ -11139,7 +11113,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="23" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B16" s="16">
         <f>B11</f>
@@ -11155,7 +11129,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="23" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B17" s="16">
         <f>'EIA Costs'!E16*About!$A$63</f>
@@ -11182,7 +11156,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11248,13 +11222,13 @@
         <v>123</v>
       </c>
       <c r="O1" s="51" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="P1" s="51" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="Q1" s="51" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -11283,7 +11257,7 @@
       </c>
       <c r="G2" s="20">
         <f>'Start Year Wind and Solar'!B7*10^6/About!$C$25*About!$A$63</f>
-        <v>1106952.27008149</v>
+        <v>1166557.3923166473</v>
       </c>
       <c r="H2" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$63</f>

</xml_diff>

<commit_message>
Recalibrated elec/ARpUIiRC for new EIA data; Used new Brattle data for elec/DRC; updated EIA data in elec/DRCo; made correction in About tab of elec/CCaMC.
</commit_message>
<xml_diff>
--- a/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
+++ b/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="230">
   <si>
     <t>Onshore Wind</t>
   </si>
@@ -734,45 +734,6 @@
   </si>
   <si>
     <t>AEO 2019</t>
-  </si>
-  <si>
-    <t>AEO 2020</t>
-  </si>
-  <si>
-    <t>AEO 2021</t>
-  </si>
-  <si>
-    <t>AEO 2022</t>
-  </si>
-  <si>
-    <t>AEO 2023</t>
-  </si>
-  <si>
-    <t>AEO 2024</t>
-  </si>
-  <si>
-    <t>AEO 2025</t>
-  </si>
-  <si>
-    <t>AEO 2026</t>
-  </si>
-  <si>
-    <t>AEO 2027</t>
-  </si>
-  <si>
-    <t>AEO 2028</t>
-  </si>
-  <si>
-    <t>AEO 2029</t>
-  </si>
-  <si>
-    <t>AEO 2030</t>
-  </si>
-  <si>
-    <t>AEO 2031</t>
-  </si>
-  <si>
-    <t>AEO 2032</t>
   </si>
   <si>
     <t>2015, 2019</t>
@@ -1723,6 +1684,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1746,9 +1710,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="228">
@@ -2340,19 +2301,19 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="78.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="56.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10.7109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.1328125" style="2"/>
+    <col min="2" max="2" width="78.59765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.3984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="77.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="56.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.73046875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2379,7 +2340,7 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="15" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="E5" s="8"/>
     </row>
@@ -2393,7 +2354,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="2" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="D7" s="2">
         <v>2018</v>
@@ -2401,10 +2362,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2412,15 +2373,15 @@
         <v>55</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2432,7 +2393,7 @@
         <v>124</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2456,7 +2417,7 @@
         <v>126</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2464,7 +2425,7 @@
         <v>127</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2481,7 +2442,7 @@
       <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="64"/>
+      <c r="D19" s="56"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="7"/>
@@ -2503,21 +2464,21 @@
       </c>
       <c r="D22" s="23"/>
     </row>
-    <row r="23" spans="1:11" ht="45">
+    <row r="23" spans="1:11" ht="42.75">
       <c r="A23" s="7"/>
       <c r="B23" s="50" t="s">
         <v>69</v>
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1">
+    <row r="24" spans="1:11" ht="14.65" thickBot="1">
       <c r="A24" s="7"/>
       <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D24" s="23"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1">
+    <row r="25" spans="1:11" ht="14.65" thickBot="1">
       <c r="A25" s="7"/>
       <c r="B25" s="21" t="s">
         <v>29</v>
@@ -2562,7 +2523,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="10" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="11"/>
@@ -2575,7 +2536,7 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="10" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="11"/>
@@ -2651,7 +2612,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="10" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="11"/>
@@ -2915,7 +2876,7 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="10" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="B58" s="9"/>
       <c r="D58" s="7"/>
@@ -2929,7 +2890,7 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="10" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="B59" s="9"/>
       <c r="D59" s="7"/>
@@ -3269,17 +3230,17 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.73046875" customWidth="1"/>
+    <col min="2" max="2" width="26.73046875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="52.59765625" customWidth="1"/>
+    <col min="4" max="4" width="34.3984375" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3380,7 +3341,7 @@
         <v>11.33</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H4" s="53">
         <v>2018</v>
@@ -3406,7 +3367,7 @@
         <v>10.3</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H5" s="53">
         <v>2018</v>
@@ -3432,7 +3393,7 @@
         <v>18.03</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H6" s="53">
         <v>2018</v>
@@ -3458,7 +3419,7 @@
         <v>7.01</v>
       </c>
       <c r="G7" s="53" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H7" s="53">
         <v>2018</v>
@@ -3484,7 +3445,7 @@
         <v>103.31</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H8" s="53">
         <v>2018</v>
@@ -3510,7 +3471,7 @@
         <v>114.39</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H9" s="53">
         <v>2018</v>
@@ -3536,7 +3497,7 @@
         <v>122.28</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H10" s="53">
         <v>2018</v>
@@ -3562,7 +3523,7 @@
         <v>40.85</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="H11" s="53">
         <v>2018</v>
@@ -3588,7 +3549,7 @@
         <v>48.42</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="H12" s="53">
         <v>2018</v>
@@ -3614,7 +3575,7 @@
         <v>80.14</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="H13" s="53">
         <v>2018</v>
@@ -3640,7 +3601,7 @@
         <v>72.84</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="H14" s="53">
         <v>2018</v>
@@ -3666,7 +3627,7 @@
         <v>22.46</v>
       </c>
       <c r="G15" s="53" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="H15" s="53">
         <v>2018</v>
@@ -3692,7 +3653,7 @@
         <v>425.38</v>
       </c>
       <c r="G16" s="53" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="H16" s="53">
         <v>2018</v>
@@ -3721,10 +3682,10 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="19" customFormat="1">
@@ -3787,11 +3748,11 @@
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" style="47" customWidth="1"/>
+    <col min="1" max="2" width="20.73046875" style="47" customWidth="1"/>
     <col min="3" max="3" width="21" style="47" customWidth="1"/>
-    <col min="4" max="8" width="20.7109375" style="47" customWidth="1"/>
+    <col min="4" max="8" width="20.73046875" style="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3816,43 +3777,43 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45">
+    <row r="2" spans="1:8" ht="27.75">
       <c r="A2" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="57" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8">
       <c r="A3" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="57"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="27" t="s">
@@ -3868,7 +3829,7 @@
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:8" ht="28.5">
+    <row r="5" spans="1:8" ht="27">
       <c r="A5" s="30" t="s">
         <v>85</v>
       </c>
@@ -3894,7 +3855,7 @@
         <v>2848907</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5">
+    <row r="6" spans="1:8" ht="27">
       <c r="A6" s="32" t="s">
         <v>86</v>
       </c>
@@ -3932,7 +3893,7 @@
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
     </row>
-    <row r="8" spans="1:8" ht="28.5">
+    <row r="8" spans="1:8" ht="27">
       <c r="A8" s="36" t="s">
         <v>88</v>
       </c>
@@ -3996,7 +3957,7 @@
         <v>30210</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="27.75">
       <c r="A11" s="39" t="s">
         <v>117</v>
       </c>
@@ -4034,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="42.75">
+    <row r="13" spans="1:8" ht="40.5">
       <c r="A13" s="36" t="s">
         <v>91</v>
       </c>
@@ -4112,7 +4073,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.5">
+    <row r="16" spans="1:8" ht="27">
       <c r="A16" s="36" t="s">
         <v>94</v>
       </c>
@@ -4138,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28.5">
+    <row r="17" spans="1:8">
       <c r="A17" s="36" t="s">
         <v>95</v>
       </c>
@@ -4164,7 +4125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28.5">
+    <row r="18" spans="1:8">
       <c r="A18" s="36" t="s">
         <v>96</v>
       </c>
@@ -4242,7 +4203,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="28.5">
+    <row r="21" spans="1:8" ht="27">
       <c r="A21" s="36" t="s">
         <v>99</v>
       </c>
@@ -4450,7 +4411,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.5">
+    <row r="29" spans="1:8" ht="27">
       <c r="A29" s="32" t="s">
         <v>109</v>
       </c>
@@ -4476,7 +4437,7 @@
         <v>35878</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28.5">
+    <row r="30" spans="1:8" ht="27">
       <c r="A30" s="43" t="s">
         <v>109</v>
       </c>
@@ -4562,15 +4523,15 @@
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="23" customWidth="1"/>
+    <col min="1" max="1" width="32.73046875" customWidth="1"/>
+    <col min="2" max="2" width="28.86328125" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="23" customFormat="1">
       <c r="A1" s="55" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -9011,7 +8972,7 @@
     <row r="42" spans="1:36" s="23" customFormat="1"/>
     <row r="43" spans="1:36" s="53" customFormat="1">
       <c r="A43" s="55" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B43" s="55"/>
     </row>
@@ -9142,7 +9103,7 @@
     <row r="60" spans="1:35" s="53" customFormat="1"/>
     <row r="61" spans="1:35" s="23" customFormat="1">
       <c r="A61" s="55" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="B61" s="54"/>
       <c r="C61" s="54"/>
@@ -10566,15 +10527,15 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.265625" customWidth="1"/>
+    <col min="2" max="2" width="23.1328125" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -10865,11 +10826,11 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="33.265625" style="23" customWidth="1"/>
     <col min="2" max="4" width="24" style="23" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="23"/>
+    <col min="5" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11159,26 +11120,26 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.265625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="4" max="5" width="17.265625" customWidth="1"/>
+    <col min="6" max="6" width="23.1328125" customWidth="1"/>
+    <col min="7" max="7" width="17.265625" customWidth="1"/>
+    <col min="8" max="8" width="22.59765625" customWidth="1"/>
+    <col min="9" max="9" width="17.265625" customWidth="1"/>
+    <col min="10" max="10" width="22.3984375" customWidth="1"/>
+    <col min="11" max="11" width="20.86328125" customWidth="1"/>
+    <col min="12" max="12" width="28.1328125" customWidth="1"/>
+    <col min="13" max="13" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.265625" customWidth="1"/>
+    <col min="16" max="16" width="18.86328125" customWidth="1"/>
+    <col min="17" max="17" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30">
+    <row r="1" spans="1:17" ht="28.5">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Permit users to override endogenous learning calculations by specifying time series capital costs in elec/CCaMC (#58)
</commit_message>
<xml_diff>
--- a/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
+++ b/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\elec\CCaMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A2D992-1D13-4349-8BC3-A9A14BCC5D04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D5C391-9B6B-41D8-9947-7A9F2F8329BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="225" windowWidth="25050" windowHeight="16770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="239">
   <si>
     <t>Onshore Wind</t>
   </si>
@@ -198,12 +198,6 @@
     <t>Except for wind and solar PV, our general approach is to take start year capital costs from the EIA and</t>
   </si>
   <si>
-    <t>Wind and Solar PV are handled differently in the model, relying on endogenous, capacity-based learning</t>
-  </si>
-  <si>
-    <t>costs, as EIA's numbers are higher than what was actually observed, so we use sources from Lawrence</t>
-  </si>
-  <si>
     <t>because the EPA's Aug 2015 rule requires new coal plants to achieve CO2 emissions no higher than</t>
   </si>
   <si>
@@ -229,9 +223,6 @@
   </si>
   <si>
     <t>For coal, we use values for a coal plant that features carbon capture and sequestration (CCS),</t>
-  </si>
-  <si>
-    <t>and the model handles calculations for subsequent years.  (We do not use EIA for the start year solar and wind</t>
   </si>
   <si>
     <t>Model Power Plant Quality</t>
@@ -600,9 +591,6 @@
     <t>Gas-CT-AvgCF - Low</t>
   </si>
   <si>
-    <t>curves to determine cost declines.  Therefore, we only specify the first simulated year costs in this spreadsheet,</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -744,9 +732,6 @@
     <t>so we assume they are 2018 dollars.</t>
   </si>
   <si>
-    <t>Berkeley National Lab and Solar Energy Industries Association.)</t>
-  </si>
-  <si>
     <t>cause them to decline at the same rate as costs declined in projections in the NREL</t>
   </si>
   <si>
@@ -805,6 +790,42 @@
   </si>
   <si>
     <t>This document is included as Appendix B of a report by Brattle Group.  It is on page 10 of the EnerNex report, which is page 70 of the PDF.</t>
+  </si>
+  <si>
+    <t>Onshore wind, offshore wind, and solar PV may optionally be handled differently in the model,</t>
+  </si>
+  <si>
+    <t>relying on endogenous, capacity-based learning curves to determine cost declines.</t>
+  </si>
+  <si>
+    <t>A cost of zero for onshore wind, offshore wind, or solar PV is a flag to the model to use endogenous</t>
+  </si>
+  <si>
+    <t>For the U.S. EPA, we do not use EIA for the start year solar and wind costs,</t>
+  </si>
+  <si>
+    <t>as EIA's numbers are higher than what was actually observed, so we use other sources,</t>
+  </si>
+  <si>
+    <t>specified above.</t>
+  </si>
+  <si>
+    <t>To use endogenous learning, you must specify a cost for the first simulated year in sheet</t>
+  </si>
+  <si>
+    <t>CCaMC-BCCpUC and leave the costs for all subsequent years set to zero.</t>
+  </si>
+  <si>
+    <t>Endogenous Learning</t>
+  </si>
+  <si>
+    <t>learning.  If a non-zero cost is provided in this sheet for a year after the first year, the model will</t>
+  </si>
+  <si>
+    <t>use the cost specified here, rather than a value calculated via endogenous learning.</t>
+  </si>
+  <si>
+    <t>Additional Notes</t>
   </si>
 </sst>
 </file>
@@ -1566,7 +1587,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1742,6 +1763,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="228">
@@ -2364,7 +2391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2400,11 +2427,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="15" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E5" s="8"/>
     </row>
@@ -2418,7 +2445,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D7" s="2">
         <v>2018</v>
@@ -2426,10 +2453,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2437,15 +2464,15 @@
         <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2454,18 +2481,18 @@
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2478,23 +2505,23 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="B17" s="23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D17" s="19"/>
     </row>
@@ -2511,7 +2538,7 @@
     <row r="20" spans="1:11">
       <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20" s="23"/>
     </row>
@@ -2524,21 +2551,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="23"/>
     </row>
     <row r="23" spans="1:11" ht="45">
       <c r="A23" s="7"/>
       <c r="B23" s="50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1">
       <c r="A24" s="7"/>
       <c r="B24" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D24" s="23"/>
     </row>
@@ -2587,7 +2614,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="10" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="11"/>
@@ -2600,7 +2627,7 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="10" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="11"/>
@@ -2623,8 +2650,8 @@
       <c r="K32" s="11"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="10" t="s">
-        <v>53</v>
+      <c r="A33" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="11"/>
@@ -2637,7 +2664,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="10" t="s">
-        <v>163</v>
+        <v>227</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="11"/>
@@ -2650,7 +2677,7 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="10" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="11"/>
@@ -2662,9 +2689,10 @@
       <c r="K35" s="11"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="A36" s="72" t="s">
+        <v>233</v>
+      </c>
+      <c r="B36" s="73"/>
       <c r="D36" s="7"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -2675,9 +2703,10 @@
       <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="10" t="s">
-        <v>211</v>
-      </c>
+      <c r="A37" s="72" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" s="73"/>
       <c r="D37" s="7"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -2688,7 +2717,9 @@
       <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="10"/>
+      <c r="A38" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="D38" s="7"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -2700,7 +2731,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="10" t="s">
-        <v>30</v>
+        <v>236</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="11"/>
@@ -2713,7 +2744,7 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="10" t="s">
-        <v>31</v>
+        <v>237</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="11"/>
@@ -2736,8 +2767,8 @@
       <c r="K41" s="11"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="10" t="s">
-        <v>63</v>
+      <c r="A42" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="11"/>
@@ -2750,7 +2781,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="10" t="s">
-        <v>55</v>
+        <v>230</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="11"/>
@@ -2763,7 +2794,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="10" t="s">
-        <v>56</v>
+        <v>231</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="11"/>
@@ -2776,7 +2807,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="10" t="s">
-        <v>57</v>
+        <v>232</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="11"/>
@@ -2788,9 +2819,7 @@
       <c r="K45" s="11"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="A46" s="10"/>
       <c r="D46" s="7"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
@@ -2802,7 +2831,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="10" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="11"/>
@@ -2814,7 +2843,9 @@
       <c r="K47" s="11"/>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="10"/>
+      <c r="A48" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="D48" s="7"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
@@ -2825,9 +2856,7 @@
       <c r="K48" s="11"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="10" t="s">
-        <v>121</v>
-      </c>
+      <c r="A49" s="10"/>
       <c r="D49" s="7"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
@@ -2839,7 +2868,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="10" t="s">
-        <v>122</v>
+        <v>61</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="11"/>
@@ -2852,7 +2881,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="10" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="11"/>
@@ -2864,7 +2893,9 @@
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="10"/>
+      <c r="A52" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="D52" s="7"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
@@ -2876,7 +2907,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="10" t="s">
-        <v>201</v>
+        <v>55</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="11"/>
@@ -2889,7 +2920,7 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="10" t="s">
-        <v>202</v>
+        <v>56</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="11"/>
@@ -2901,7 +2932,9 @@
       <c r="K54" s="11"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="10"/>
+      <c r="A55" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="D55" s="7"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -2912,9 +2945,7 @@
       <c r="K55" s="11"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="A56" s="10"/>
       <c r="D56" s="7"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
@@ -2926,9 +2957,8 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" s="9"/>
+        <v>118</v>
+      </c>
       <c r="D57" s="7"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
@@ -2940,9 +2970,8 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B58" s="9"/>
+        <v>119</v>
+      </c>
       <c r="D58" s="7"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
@@ -2954,9 +2983,8 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B59" s="9"/>
+        <v>120</v>
+      </c>
       <c r="D59" s="7"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
@@ -2967,10 +2995,7 @@
       <c r="K59" s="11"/>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="9"/>
+      <c r="A60" s="10"/>
       <c r="D60" s="7"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -2981,10 +3006,9 @@
       <c r="K60" s="11"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="19">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="B61" s="9"/>
+      <c r="A61" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="D61" s="7"/>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
@@ -2995,10 +3019,9 @@
       <c r="K61" s="11"/>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B62" s="9"/>
+      <c r="A62" s="10" t="s">
+        <v>198</v>
+      </c>
       <c r="D62" s="7"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -3009,10 +3032,7 @@
       <c r="K62" s="11"/>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="25">
-        <v>0.9143</v>
-      </c>
-      <c r="B63" s="9"/>
+      <c r="A63" s="10"/>
       <c r="D63" s="7"/>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
@@ -3023,10 +3043,9 @@
       <c r="K63" s="11"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B64" s="9"/>
+      <c r="A64" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="D64" s="7"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -3037,8 +3056,8 @@
       <c r="K64" s="11"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="25">
-        <v>0.89800000000000002</v>
+      <c r="A65" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="B65" s="9"/>
       <c r="D65" s="7"/>
@@ -3051,7 +3070,9 @@
       <c r="K65" s="11"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="25"/>
+      <c r="A66" s="10" t="s">
+        <v>205</v>
+      </c>
       <c r="B66" s="9"/>
       <c r="D66" s="7"/>
       <c r="E66" s="11"/>
@@ -3063,8 +3084,8 @@
       <c r="K66" s="11"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="19" t="s">
-        <v>24</v>
+      <c r="A67" s="10" t="s">
+        <v>206</v>
       </c>
       <c r="B67" s="9"/>
       <c r="D67" s="7"/>
@@ -3077,7 +3098,9 @@
       <c r="K67" s="11"/>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="10"/>
+      <c r="A68" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="B68" s="9"/>
       <c r="D68" s="7"/>
       <c r="E68" s="11"/>
@@ -3089,7 +3112,9 @@
       <c r="K68" s="11"/>
     </row>
     <row r="69" spans="1:11">
-      <c r="A69" s="10"/>
+      <c r="A69" s="19">
+        <v>0.98599999999999999</v>
+      </c>
       <c r="B69" s="9"/>
       <c r="D69" s="7"/>
       <c r="E69" s="11"/>
@@ -3101,7 +3126,9 @@
       <c r="K69" s="11"/>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="10"/>
+      <c r="A70" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="B70" s="9"/>
       <c r="D70" s="7"/>
       <c r="E70" s="11"/>
@@ -3113,7 +3140,9 @@
       <c r="K70" s="11"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="10"/>
+      <c r="A71" s="25">
+        <v>0.9143</v>
+      </c>
       <c r="B71" s="9"/>
       <c r="D71" s="7"/>
       <c r="E71" s="11"/>
@@ -3125,7 +3154,9 @@
       <c r="K71" s="11"/>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="10"/>
+      <c r="A72" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="B72" s="9"/>
       <c r="D72" s="7"/>
       <c r="E72" s="11"/>
@@ -3137,7 +3168,9 @@
       <c r="K72" s="11"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="10"/>
+      <c r="A73" s="25">
+        <v>0.89800000000000002</v>
+      </c>
       <c r="B73" s="9"/>
       <c r="D73" s="7"/>
       <c r="E73" s="11"/>
@@ -3149,7 +3182,7 @@
       <c r="K73" s="11"/>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="10"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="9"/>
       <c r="D74" s="7"/>
       <c r="E74" s="11"/>
@@ -3161,7 +3194,9 @@
       <c r="K74" s="11"/>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="10"/>
+      <c r="A75" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="B75" s="9"/>
       <c r="D75" s="7"/>
       <c r="E75" s="11"/>
@@ -3293,7 +3328,7 @@
       <c r="K85" s="11"/>
     </row>
     <row r="86" spans="1:11">
-      <c r="A86" s="7"/>
+      <c r="A86" s="10"/>
       <c r="B86" s="9"/>
       <c r="D86" s="7"/>
       <c r="E86" s="11"/>
@@ -3303,6 +3338,102 @@
       <c r="I86" s="11"/>
       <c r="J86" s="11"/>
       <c r="K86" s="11"/>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" s="10"/>
+      <c r="B87" s="9"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="11"/>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88" s="10"/>
+      <c r="B88" s="9"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="11"/>
+      <c r="K88" s="11"/>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" s="10"/>
+      <c r="B89" s="9"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
+      <c r="K89" s="11"/>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="10"/>
+      <c r="B90" s="9"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11"/>
+      <c r="I90" s="11"/>
+      <c r="J90" s="11"/>
+      <c r="K90" s="11"/>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" s="10"/>
+      <c r="B91" s="9"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="11"/>
+      <c r="I91" s="11"/>
+      <c r="J91" s="11"/>
+      <c r="K91" s="11"/>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" s="10"/>
+      <c r="B92" s="9"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="11"/>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" s="10"/>
+      <c r="B93" s="9"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="11"/>
+      <c r="J93" s="11"/>
+      <c r="K93" s="11"/>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" s="7"/>
+      <c r="B94" s="9"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="11"/>
+      <c r="K94" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3340,36 +3471,36 @@
         <v>41</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" s="57" t="s">
         <v>43</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>22</v>
       </c>
       <c r="F1" s="51" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G1" s="59" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I1" s="57" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
@@ -3387,21 +3518,21 @@
         <v>2013</v>
       </c>
       <c r="H2" s="61" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D3" s="63">
         <v>4652</v>
@@ -3416,7 +3547,7 @@
         <v>2019</v>
       </c>
       <c r="H3" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3424,7 +3555,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
@@ -3442,10 +3573,10 @@
         <v>2018</v>
       </c>
       <c r="H4" s="61" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I4" s="53" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3453,10 +3584,10 @@
         <v>33</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D5" s="63">
         <v>1079</v>
@@ -3471,7 +3602,7 @@
         <v>2019</v>
       </c>
       <c r="H5" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3479,7 +3610,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
@@ -3497,10 +3628,10 @@
         <v>2018</v>
       </c>
       <c r="H6" s="61" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I6" s="53" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3508,10 +3639,10 @@
         <v>36</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D7" s="63">
         <v>710</v>
@@ -3526,7 +3657,7 @@
         <v>2019</v>
       </c>
       <c r="H7" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3534,7 +3665,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
         <v>46</v>
@@ -3552,7 +3683,7 @@
         <v>2019</v>
       </c>
       <c r="H8" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3560,7 +3691,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -3578,7 +3709,7 @@
         <v>2019</v>
       </c>
       <c r="H9" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3586,7 +3717,7 @@
         <v>34</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
@@ -3604,7 +3735,7 @@
         <v>2019</v>
       </c>
       <c r="H10" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3612,7 +3743,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
@@ -3630,15 +3761,15 @@
         <v>2019</v>
       </c>
       <c r="H11" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -3656,15 +3787,15 @@
         <v>2019</v>
       </c>
       <c r="H12" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>48</v>
@@ -3682,7 +3813,7 @@
         <v>2019</v>
       </c>
       <c r="H13" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3690,7 +3821,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -3708,7 +3839,7 @@
         <v>2019</v>
       </c>
       <c r="H14" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3716,7 +3847,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>49</v>
@@ -3734,18 +3865,18 @@
         <v>2019</v>
       </c>
       <c r="H15" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="23" customFormat="1">
       <c r="A16" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>196</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>200</v>
       </c>
       <c r="D16" s="52">
         <v>1557</v>
@@ -3760,7 +3891,7 @@
         <v>2019</v>
       </c>
       <c r="H16" s="63" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3768,12 +3899,12 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -3796,7 +3927,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="19" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="19" customFormat="1">
@@ -3818,7 +3949,7 @@
     <row r="4" spans="1:2" s="19" customFormat="1"/>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="19" customFormat="1">
@@ -3865,53 +3996,53 @@
       <c r="A1" s="26"/>
       <c r="B1" s="26"/>
       <c r="C1" s="27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45">
       <c r="A2" s="28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="66" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="G2" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="70" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="70" t="s">
-        <v>106</v>
-      </c>
       <c r="H2" s="64" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30">
       <c r="A3" s="27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="67"/>
       <c r="C3" s="69"/>
@@ -3923,7 +4054,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="29">
         <v>1000</v>
@@ -3937,7 +4068,7 @@
     </row>
     <row r="5" spans="1:8" ht="28.5">
       <c r="A5" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="29">
         <v>1000</v>
@@ -3963,10 +4094,10 @@
     </row>
     <row r="6" spans="1:8" ht="28.5">
       <c r="A6" s="32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" s="33">
         <v>3641</v>
@@ -3989,7 +4120,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -4001,7 +4132,7 @@
     </row>
     <row r="8" spans="1:8" ht="28.5">
       <c r="A8" s="36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B8" s="37">
         <v>1000</v>
@@ -4027,7 +4158,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="39" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
@@ -4039,7 +4170,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" s="37">
         <v>1000</v>
@@ -4065,7 +4196,7 @@
     </row>
     <row r="11" spans="1:8" ht="30">
       <c r="A11" s="39" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B11" s="35"/>
       <c r="C11" s="35"/>
@@ -4077,7 +4208,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B12" s="37">
         <v>1000</v>
@@ -4103,7 +4234,7 @@
     </row>
     <row r="13" spans="1:8" ht="42.75">
       <c r="A13" s="36" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B13" s="37">
         <v>1000</v>
@@ -4129,7 +4260,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B14" s="37">
         <v>1000</v>
@@ -4155,7 +4286,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B15" s="37">
         <v>1000</v>
@@ -4181,7 +4312,7 @@
     </row>
     <row r="16" spans="1:8" ht="28.5">
       <c r="A16" s="36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B16" s="37">
         <v>1000</v>
@@ -4207,7 +4338,7 @@
     </row>
     <row r="17" spans="1:8" ht="28.5">
       <c r="A17" s="36" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B17" s="37">
         <v>1000</v>
@@ -4233,7 +4364,7 @@
     </row>
     <row r="18" spans="1:8" ht="28.5">
       <c r="A18" s="36" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B18" s="37">
         <v>1000</v>
@@ -4259,7 +4390,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="36" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B19" s="37">
         <v>1000</v>
@@ -4285,7 +4416,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="36" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B20" s="37">
         <v>1000</v>
@@ -4311,7 +4442,7 @@
     </row>
     <row r="21" spans="1:8" ht="28.5">
       <c r="A21" s="36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B21" s="37">
         <v>1000</v>
@@ -4337,7 +4468,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B22" s="37">
         <v>1000</v>
@@ -4363,7 +4494,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B23" s="37">
         <v>1000</v>
@@ -4389,7 +4520,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B24" s="37">
         <v>1000</v>
@@ -4415,7 +4546,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B25" s="37">
         <v>1000</v>
@@ -4441,19 +4572,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="36" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B26" s="37">
         <v>1000</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F26" s="41">
         <v>555</v>
@@ -4467,7 +4598,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B27" s="37">
         <v>1000</v>
@@ -4493,10 +4624,10 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="43" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C28" s="44">
         <v>3.73</v>
@@ -4519,7 +4650,7 @@
     </row>
     <row r="29" spans="1:8" ht="28.5">
       <c r="A29" s="32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B29" s="45">
         <v>1000</v>
@@ -4545,10 +4676,10 @@
     </row>
     <row r="30" spans="1:8" ht="28.5">
       <c r="A30" s="43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C30" s="44">
         <v>7.69</v>
@@ -4571,12 +4702,12 @@
     </row>
     <row r="32" spans="1:8">
       <c r="B32" s="47" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="48" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B33" s="49">
         <f>D6/AVERAGE(C6,E6)</f>
@@ -4587,7 +4718,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="48" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B34" s="49">
         <f>D28/(AVERAGE(C28,E28))</f>
@@ -4598,7 +4729,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B35" s="49">
         <f>D10/AVERAGE(E10,C10)</f>
@@ -4637,7 +4768,7 @@
   <sheetData>
     <row r="1" spans="1:36" s="23" customFormat="1">
       <c r="A1" s="55" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -4677,10 +4808,10 @@
     </row>
     <row r="2" spans="1:36" s="23" customFormat="1">
       <c r="A2" s="23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C2" s="23">
         <v>2017</v>
@@ -4790,7 +4921,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C3" s="53">
         <v>5179.5016296472777</v>
@@ -4900,7 +5031,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C4" s="53">
         <v>906.43752501948961</v>
@@ -5010,7 +5141,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C5" s="53">
         <v>6044.2528846388041</v>
@@ -5120,7 +5251,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C6" s="53">
         <v>5501.4276276478286</v>
@@ -5230,7 +5361,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C7" s="53">
         <v>4068.8324979159847</v>
@@ -5340,7 +5471,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C8" s="53">
         <v>3836.1961011946664</v>
@@ -5450,7 +5581,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C9" s="53">
         <v>7123.1024412096613</v>
@@ -5560,7 +5691,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C10" s="53">
         <v>6358.970494457717</v>
@@ -5670,7 +5801,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C11" s="53">
         <v>6228.2456569988753</v>
@@ -5780,7 +5911,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C12" s="53">
         <v>5606.8362940961097</v>
@@ -5890,7 +6021,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C13" s="53">
         <v>6199.7160723985862</v>
@@ -6000,7 +6131,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C14" s="53">
         <v>7561.0934235746954</v>
@@ -6110,7 +6241,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C15" s="53">
         <v>7561.0934235746954</v>
@@ -6220,7 +6351,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C16" s="53">
         <v>7561.0934235746954</v>
@@ -6330,7 +6461,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C17" s="53">
         <v>3827.2968566587979</v>
@@ -6440,7 +6571,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C18" s="53">
         <v>4013.1693740693227</v>
@@ -6550,7 +6681,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C19" s="53">
         <v>4013.1693740693227</v>
@@ -6660,7 +6791,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C20" s="53">
         <v>4305.3925876948315</v>
@@ -6770,7 +6901,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C21" s="53">
         <v>5576.5909167824766</v>
@@ -6880,7 +7011,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C22" s="53">
         <v>14196.524804379835</v>
@@ -6990,7 +7121,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C23" s="53">
         <v>31389.002895326357</v>
@@ -7100,7 +7231,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C24" s="53">
         <v>14196.524804379835</v>
@@ -7210,7 +7341,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C25" s="53">
         <v>31389.002895326357</v>
@@ -7320,7 +7451,7 @@
         <v>36</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C26" s="53">
         <v>899.1125440742336</v>
@@ -7427,10 +7558,10 @@
     </row>
     <row r="27" spans="1:36">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C27" s="53">
         <v>2985.7163232225957</v>
@@ -7537,10 +7668,10 @@
     </row>
     <row r="28" spans="1:36">
       <c r="A28" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C28" s="53">
         <v>3068.5330578578878</v>
@@ -7647,10 +7778,10 @@
     </row>
     <row r="29" spans="1:36">
       <c r="A29" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C29" s="53">
         <v>3161.5232415013843</v>
@@ -7757,10 +7888,10 @@
     </row>
     <row r="30" spans="1:36">
       <c r="A30" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C30" s="53">
         <v>3433.5732515006521</v>
@@ -7867,10 +7998,10 @@
     </row>
     <row r="31" spans="1:36">
       <c r="A31" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C31" s="53">
         <v>3650.4675562858592</v>
@@ -7977,10 +8108,10 @@
     </row>
     <row r="32" spans="1:36">
       <c r="A32" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C32" s="53">
         <v>4469.1889883621543</v>
@@ -8087,10 +8218,10 @@
     </row>
     <row r="33" spans="1:36">
       <c r="A33" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C33" s="53">
         <v>4351.9349981933547</v>
@@ -8197,10 +8328,10 @@
     </row>
     <row r="34" spans="1:36">
       <c r="A34" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C34" s="53">
         <v>4362.9480041823535</v>
@@ -8307,10 +8438,10 @@
     </row>
     <row r="35" spans="1:36">
       <c r="A35" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C35" s="53">
         <v>4522.3633673455815</v>
@@ -8417,10 +8548,10 @@
     </row>
     <row r="36" spans="1:36">
       <c r="A36" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C36" s="53">
         <v>4645.8187533874998</v>
@@ -8527,10 +8658,10 @@
     </row>
     <row r="37" spans="1:36">
       <c r="A37" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C37" s="53">
         <v>4654.7690040318539</v>
@@ -8637,10 +8768,10 @@
     </row>
     <row r="38" spans="1:36" s="23" customFormat="1">
       <c r="A38" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C38" s="53">
         <v>4598.9063450796984</v>
@@ -8747,10 +8878,10 @@
     </row>
     <row r="39" spans="1:36" s="23" customFormat="1">
       <c r="A39" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C39" s="53">
         <v>4826.7338115915436</v>
@@ -8857,10 +8988,10 @@
     </row>
     <row r="40" spans="1:36" s="23" customFormat="1">
       <c r="A40" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C40" s="53">
         <v>4996.613495139718</v>
@@ -8967,10 +9098,10 @@
     </row>
     <row r="41" spans="1:36" s="23" customFormat="1">
       <c r="A41" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C41" s="53">
         <v>5256.8000129437169</v>
@@ -9078,7 +9209,7 @@
     <row r="42" spans="1:36" s="23" customFormat="1"/>
     <row r="43" spans="1:36" s="53" customFormat="1">
       <c r="A43" s="55" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B43" s="55"/>
     </row>
@@ -9088,7 +9219,7 @@
     </row>
     <row r="45" spans="1:36" s="53" customFormat="1">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B45" s="23">
         <v>12.491269722013936</v>
@@ -9096,7 +9227,7 @@
     </row>
     <row r="46" spans="1:36" s="53" customFormat="1">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B46" s="23">
         <v>24.982539444027871</v>
@@ -9104,7 +9235,7 @@
     </row>
     <row r="47" spans="1:36" s="53" customFormat="1">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B47" s="23">
         <v>49.965078888055743</v>
@@ -9112,7 +9243,7 @@
     </row>
     <row r="48" spans="1:36" s="53" customFormat="1">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B48" s="23">
         <v>320</v>
@@ -9120,7 +9251,7 @@
     </row>
     <row r="49" spans="1:35" s="53" customFormat="1">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B49" s="23">
         <v>320</v>
@@ -9128,7 +9259,7 @@
     </row>
     <row r="50" spans="1:35" s="53" customFormat="1">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B50" s="23">
         <v>12.491269722013936</v>
@@ -9136,7 +9267,7 @@
     </row>
     <row r="51" spans="1:35" s="53" customFormat="1">
       <c r="A51" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B51" s="23">
         <v>24.982539444027871</v>
@@ -9144,7 +9275,7 @@
     </row>
     <row r="52" spans="1:35" s="53" customFormat="1">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B52" s="23">
         <v>49.965078888055743</v>
@@ -9152,7 +9283,7 @@
     </row>
     <row r="53" spans="1:35" s="53" customFormat="1">
       <c r="A53" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B53" s="23">
         <v>99.930157776111486</v>
@@ -9160,7 +9291,7 @@
     </row>
     <row r="54" spans="1:35" s="53" customFormat="1">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B54" s="23">
         <v>199.86031555222297</v>
@@ -9168,7 +9299,7 @@
     </row>
     <row r="55" spans="1:35" s="53" customFormat="1">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B55" s="23">
         <v>199.86031555222297</v>
@@ -9176,7 +9307,7 @@
     </row>
     <row r="56" spans="1:35" s="53" customFormat="1">
       <c r="A56" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B56" s="23">
         <v>199.86031555222297</v>
@@ -9184,7 +9315,7 @@
     </row>
     <row r="57" spans="1:35" s="53" customFormat="1">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B57" s="23">
         <v>199.86031555222297</v>
@@ -9192,7 +9323,7 @@
     </row>
     <row r="58" spans="1:35" s="53" customFormat="1">
       <c r="A58" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B58" s="23">
         <v>199.86031555222297</v>
@@ -9200,7 +9331,7 @@
     </row>
     <row r="59" spans="1:35" s="53" customFormat="1">
       <c r="A59" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B59" s="23">
         <v>143.39977640871999</v>
@@ -9209,7 +9340,7 @@
     <row r="60" spans="1:35" s="53" customFormat="1"/>
     <row r="61" spans="1:35" s="23" customFormat="1">
       <c r="A61" s="55" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B61" s="54"/>
       <c r="C61" s="54"/>
@@ -10481,7 +10612,7 @@
     </row>
     <row r="71" spans="1:35">
       <c r="A71" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B71" s="23">
         <f t="shared" ref="B71:AI71" si="8">(SUMPRODUCT(C$27:C$41,$B$45:$B$59)/SUM($B$45:$B$59))/(SUMPRODUCT($C$27:$C$41,$B$45:$B$59)/SUM($B$45:$B$59))</f>
@@ -10647,28 +10778,28 @@
         <v>21</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>69</v>
-      </c>
       <c r="D1" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" s="4">
-        <f>('EIA Costs'!F2*1000)*(About!$A$61)</f>
+        <f>('EIA Costs'!F2*1000)*(About!$A$69)</f>
         <v>30723.759999999998</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" s="4">
-        <f>'EIA Costs'!F3*1000*About!$A$61</f>
+        <f>'EIA Costs'!F3*1000*About!$A$69</f>
         <v>53313.02</v>
       </c>
     </row>
@@ -10677,14 +10808,14 @@
         <v>33</v>
       </c>
       <c r="B3" s="4">
-        <f>('EIA Costs'!F4*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F4*1000)*(About!$A$71)</f>
         <v>10359.019</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="4">
-        <f>'EIA Costs'!F5*1000*About!$A$63</f>
+        <f>'EIA Costs'!F5*1000*About!$A$71</f>
         <v>12836.772000000001</v>
       </c>
     </row>
@@ -10693,14 +10824,14 @@
         <v>16</v>
       </c>
       <c r="B4" s="4">
-        <f>('EIA Costs'!F8*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F8*1000)*(About!$A$71)</f>
         <v>110749.159</v>
       </c>
       <c r="C4" s="23">
         <v>0</v>
       </c>
       <c r="D4" s="4">
-        <f>'EIA Costs'!F8*1000*About!$A$63</f>
+        <f>'EIA Costs'!F8*1000*About!$A$71</f>
         <v>110749.159</v>
       </c>
     </row>
@@ -10709,30 +10840,30 @@
         <v>17</v>
       </c>
       <c r="B5" s="4">
-        <f>('EIA Costs'!F11*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F11*1000)*(About!$A$71)</f>
         <v>38062.309000000001</v>
       </c>
       <c r="C5" s="23">
         <v>0</v>
       </c>
       <c r="D5" s="4">
-        <f>'EIA Costs'!F11*1000*About!$A$63</f>
+        <f>'EIA Costs'!F11*1000*About!$A$71</f>
         <v>38062.309000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B6" s="4">
-        <f>('EIA Costs'!F12*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F12*1000)*(About!$A$71)</f>
         <v>23972.946</v>
       </c>
       <c r="C6" s="23">
         <v>0</v>
       </c>
       <c r="D6" s="4">
-        <f>'EIA Costs'!F12*1000*About!$A$63</f>
+        <f>'EIA Costs'!F12*1000*About!$A$71</f>
         <v>23972.946</v>
       </c>
     </row>
@@ -10741,14 +10872,14 @@
         <v>18</v>
       </c>
       <c r="B7" s="4">
-        <f>('EIA Costs'!F15*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F15*1000)*(About!$A$71)</f>
         <v>13888.217000000001</v>
       </c>
       <c r="C7" s="23">
         <v>0</v>
       </c>
       <c r="D7" s="4">
-        <f>'EIA Costs'!F15*1000*About!$A$63</f>
+        <f>'EIA Costs'!F15*1000*About!$A$71</f>
         <v>13888.217000000001</v>
       </c>
     </row>
@@ -10757,14 +10888,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="4">
-        <f>('EIA Costs'!F14*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F14*1000)*(About!$A$71)</f>
         <v>77742.929000000004</v>
       </c>
       <c r="C8" s="23">
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <f>'EIA Costs'!F14*1000*About!$A$63</f>
+        <f>'EIA Costs'!F14*1000*About!$A$71</f>
         <v>77742.929000000004</v>
       </c>
     </row>
@@ -10773,14 +10904,14 @@
         <v>20</v>
       </c>
       <c r="B9" s="4">
-        <f>('EIA Costs'!F9*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F9*1000)*(About!$A$71)</f>
         <v>114461.217</v>
       </c>
       <c r="C9" s="23">
         <v>0</v>
       </c>
       <c r="D9" s="4">
-        <f>'EIA Costs'!F9*1000*About!$A$63</f>
+        <f>'EIA Costs'!F9*1000*About!$A$71</f>
         <v>114461.217</v>
       </c>
     </row>
@@ -10789,14 +10920,14 @@
         <v>34</v>
       </c>
       <c r="B10" s="4">
-        <f>('EIA Costs'!F10*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F10*1000)*(About!$A$71)</f>
         <v>103581.04700000001</v>
       </c>
       <c r="C10" s="23">
         <v>0</v>
       </c>
       <c r="D10" s="4">
-        <f>'EIA Costs'!F10*1000*About!$A$63</f>
+        <f>'EIA Costs'!F10*1000*About!$A$71</f>
         <v>103581.04700000001</v>
       </c>
     </row>
@@ -10805,7 +10936,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="4">
-        <f>(B12)*(About!$A$63)</f>
+        <f>(B12)*(About!$A$71)</f>
         <v>15072.079154700001</v>
       </c>
       <c r="C11" s="23">
@@ -10821,20 +10952,20 @@
         <v>36</v>
       </c>
       <c r="B12" s="4">
-        <f>('EIA Costs'!F6*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F6*1000)*(About!$A$71)</f>
         <v>16484.829000000002</v>
       </c>
       <c r="C12" s="23">
         <v>0</v>
       </c>
       <c r="D12" s="4">
-        <f>'EIA Costs'!F7*1000*About!$A$63</f>
+        <f>'EIA Costs'!F7*1000*About!$A$71</f>
         <v>6372.6710000000003</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B13" s="4">
         <f>B2*'Coal Cost Multipliers'!$B$35</f>
@@ -10851,23 +10982,23 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B14" s="4">
-        <f>('EIA Costs'!F13*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F13*1000)*(About!$A$71)</f>
         <v>100152.42200000001</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" s="4">
-        <f>'EIA Costs'!F13*1000*About!$A$63</f>
+        <f>'EIA Costs'!F13*1000*About!$A$71</f>
         <v>100152.42200000001</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B15" s="4">
         <f>B11</f>
@@ -10883,7 +11014,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B16" s="4">
         <f>B11</f>
@@ -10899,17 +11030,17 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B17" s="4">
-        <f>('EIA Costs'!F16*1000)*(About!$A$63)</f>
+        <f>('EIA Costs'!F16*1000)*(About!$A$71)</f>
         <v>18304.286</v>
       </c>
       <c r="C17" s="23">
         <v>0</v>
       </c>
       <c r="D17" s="4">
-        <f>'EIA Costs'!F16*1000*About!$A$63</f>
+        <f>'EIA Costs'!F16*1000*About!$A$71</f>
         <v>18304.286</v>
       </c>
     </row>
@@ -10940,13 +11071,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>69</v>
-      </c>
       <c r="D1" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -10954,14 +11085,14 @@
         <v>15</v>
       </c>
       <c r="B2" s="16">
-        <f>'EIA Costs'!E2*About!$A$61</f>
+        <f>'EIA Costs'!E2*About!$A$69</f>
         <v>4.4074200000000001</v>
       </c>
       <c r="C2" s="23">
         <v>0</v>
       </c>
       <c r="D2" s="16">
-        <f>'EIA Costs'!E3*About!$A$61</f>
+        <f>'EIA Costs'!E3*About!$A$69</f>
         <v>6.9512999999999998</v>
       </c>
     </row>
@@ -10970,14 +11101,14 @@
         <v>33</v>
       </c>
       <c r="B3" s="16">
-        <f>'EIA Costs'!E4*About!$A$63</f>
+        <f>'EIA Costs'!E4*About!$A$71</f>
         <v>3.3006229999999999</v>
       </c>
       <c r="C3" s="23">
         <v>0</v>
       </c>
       <c r="D3" s="16">
-        <f>'EIA Costs'!E5*About!$A$63</f>
+        <f>'EIA Costs'!E5*About!$A$71</f>
         <v>2.3223220000000002</v>
       </c>
     </row>
@@ -10986,14 +11117,14 @@
         <v>16</v>
       </c>
       <c r="B4" s="16">
-        <f>'EIA Costs'!E8*About!$A$63</f>
+        <f>'EIA Costs'!E8*About!$A$71</f>
         <v>2.1577479999999998</v>
       </c>
       <c r="C4" s="23">
         <v>0</v>
       </c>
       <c r="D4" s="16">
-        <f>'EIA Costs'!E8*About!$A$63</f>
+        <f>'EIA Costs'!E8*About!$A$71</f>
         <v>2.1577479999999998</v>
       </c>
     </row>
@@ -11002,30 +11133,30 @@
         <v>17</v>
       </c>
       <c r="B5" s="16">
-        <f>'EIA Costs'!E11*About!$A$63</f>
+        <f>'EIA Costs'!E11*About!$A$71</f>
         <v>1.2708769999999998</v>
       </c>
       <c r="C5" s="23">
         <v>0</v>
       </c>
       <c r="D5" s="16">
-        <f>'EIA Costs'!E11*About!$A$63</f>
+        <f>'EIA Costs'!E11*About!$A$71</f>
         <v>1.2708769999999998</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B6" s="4">
-        <f>'EIA Costs'!E12*About!$A$63</f>
+        <f>'EIA Costs'!E12*About!$A$71</f>
         <v>0</v>
       </c>
       <c r="C6" s="23">
         <v>0</v>
       </c>
       <c r="D6" s="4">
-        <f>'EIA Costs'!E12*About!$A$63</f>
+        <f>'EIA Costs'!E12*About!$A$71</f>
         <v>0</v>
       </c>
     </row>
@@ -11034,14 +11165,14 @@
         <v>18</v>
       </c>
       <c r="B7" s="4">
-        <f>'EIA Costs'!E15*About!$A$63</f>
+        <f>'EIA Costs'!E15*About!$A$71</f>
         <v>0</v>
       </c>
       <c r="C7" s="23">
         <v>0</v>
       </c>
       <c r="D7" s="4">
-        <f>'EIA Costs'!E15*About!$A$63</f>
+        <f>'EIA Costs'!E15*About!$A$71</f>
         <v>0</v>
       </c>
     </row>
@@ -11050,14 +11181,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="4">
-        <f>'EIA Costs'!E14*About!$A$63</f>
+        <f>'EIA Costs'!E14*About!$A$71</f>
         <v>0</v>
       </c>
       <c r="C8" s="23">
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <f>'EIA Costs'!E14*About!$A$63</f>
+        <f>'EIA Costs'!E14*About!$A$71</f>
         <v>0</v>
       </c>
     </row>
@@ -11066,14 +11197,14 @@
         <v>20</v>
       </c>
       <c r="B9" s="16">
-        <f>'EIA Costs'!E9*About!$A$63</f>
+        <f>'EIA Costs'!E9*About!$A$71</f>
         <v>4.3977829999999996</v>
       </c>
       <c r="C9" s="23">
         <v>0</v>
       </c>
       <c r="D9" s="16">
-        <f>'EIA Costs'!E9*About!$A$63</f>
+        <f>'EIA Costs'!E9*About!$A$71</f>
         <v>4.3977829999999996</v>
       </c>
     </row>
@@ -11082,14 +11213,14 @@
         <v>34</v>
       </c>
       <c r="B10" s="4">
-        <f>'EIA Costs'!E10*About!$A$63</f>
+        <f>'EIA Costs'!E10*About!$A$71</f>
         <v>1.0605879999999999</v>
       </c>
       <c r="C10" s="23">
         <v>0</v>
       </c>
       <c r="D10" s="4">
-        <f>'EIA Costs'!E10*About!$A$63</f>
+        <f>'EIA Costs'!E10*About!$A$71</f>
         <v>1.0605879999999999</v>
       </c>
     </row>
@@ -11114,20 +11245,20 @@
         <v>36</v>
       </c>
       <c r="B12" s="16">
-        <f>'EIA Costs'!E6*About!$A$63</f>
+        <f>'EIA Costs'!E6*About!$A$71</f>
         <v>3.3006229999999999</v>
       </c>
       <c r="C12" s="23">
         <v>0</v>
       </c>
       <c r="D12" s="16">
-        <f>'EIA Costs'!E7*About!$A$63</f>
+        <f>'EIA Costs'!E7*About!$A$71</f>
         <v>4.0960640000000001</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B13" s="16">
         <f>B2*'Coal Cost Multipliers'!$B$34</f>
@@ -11144,7 +11275,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B14" s="23">
         <f>'EIA Costs'!E13*1000</f>
@@ -11154,13 +11285,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="23">
-        <f>'EIA Costs'!E13*1000*About!$A$63</f>
+        <f>'EIA Costs'!E13*1000*About!$A$71</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="23" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B15" s="16">
         <f>B11</f>
@@ -11176,7 +11307,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="23" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B16" s="16">
         <f>B11</f>
@@ -11192,17 +11323,17 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="23" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B17" s="16">
-        <f>'EIA Costs'!E16*About!$A$63</f>
+        <f>'EIA Costs'!E16*About!$A$71</f>
         <v>5.6412310000000003</v>
       </c>
       <c r="C17" s="23">
         <v>0</v>
       </c>
       <c r="D17" s="16">
-        <f>'EIA Costs'!E16*About!$A$63</f>
+        <f>'EIA Costs'!E16*About!$A$71</f>
         <v>5.6412310000000003</v>
       </c>
     </row>
@@ -11244,7 +11375,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>37</v>
@@ -11256,7 +11387,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>10</v>
@@ -11277,19 +11408,19 @@
         <v>40</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="O1" s="51" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="P1" s="51" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="Q1" s="51" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -11297,47 +11428,47 @@
         <v>2018</v>
       </c>
       <c r="B2" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4557579.6788879326</v>
       </c>
       <c r="C2" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>962058.30273462704</v>
       </c>
       <c r="D2" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5632940.678707079</v>
       </c>
       <c r="E2" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2434233.6034520324</v>
       </c>
       <c r="F2" s="20">
-        <f>'Start Year Wind and Solar'!B3*10^3*About!$A$63</f>
+        <f>'Start Year Wind and Solar'!B3*10^3*About!$A$71</f>
         <v>1344021</v>
       </c>
       <c r="G2" s="20">
-        <f>'Start Year Wind and Solar'!B7*10^6/About!$C$25*About!$A$63</f>
+        <f>'Start Year Wind and Solar'!B7*10^6/About!$C$25*About!$A$71</f>
         <v>1166557.3923166473</v>
       </c>
       <c r="H2" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>6190235.3107596356</v>
       </c>
       <c r="I2" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3680479.6131787207</v>
       </c>
       <c r="J2" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2270817.9963020692</v>
       </c>
       <c r="K2" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>636580.52455604961</v>
       </c>
       <c r="L2" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>636580.52455604961</v>
       </c>
       <c r="M2" s="4">
@@ -11345,7 +11476,7 @@
         <v>5281971.7859389298</v>
       </c>
       <c r="N2" s="20">
-        <f>SUMPRODUCT('Cost Improvement and Off Wnd'!B45:B59,'Cost Improvement and Off Wnd'!C27:C41)/SUM('Cost Improvement and Off Wnd'!B45:B59)*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("offshore wind",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH(A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*10^3*About!$A$63</f>
+        <f>SUMPRODUCT('Cost Improvement and Off Wnd'!B45:B59,'Cost Improvement and Off Wnd'!C27:C41)/SUM('Cost Improvement and Off Wnd'!B45:B59)*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("offshore wind",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH(A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*10^3*About!$A$71</f>
         <v>3030248.6826914768</v>
       </c>
       <c r="O2" s="4">
@@ -11357,7 +11488,7 @@
         <v>636580.52455604961</v>
       </c>
       <c r="Q2" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1396322.3093857865</v>
       </c>
     </row>
@@ -11366,19 +11497,19 @@
         <v>2019</v>
       </c>
       <c r="B3" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4528287.3577758651</v>
       </c>
       <c r="C3" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>955174.60546925361</v>
       </c>
       <c r="D3" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5593215.3574141553</v>
       </c>
       <c r="E3" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2397171.2069040639</v>
       </c>
       <c r="F3" s="4">
@@ -11388,23 +11519,23 @@
         <v>0</v>
       </c>
       <c r="H3" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5922952.6215192685</v>
       </c>
       <c r="I3" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3675567.2263574409</v>
       </c>
       <c r="J3" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2134995.9926041379</v>
       </c>
       <c r="K3" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>635581.04911209899</v>
       </c>
       <c r="L3" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>635581.04911209899</v>
       </c>
       <c r="M3" s="4">
@@ -11423,7 +11554,7 @@
         <v>635581.04911209899</v>
       </c>
       <c r="Q3" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1394458.6187715731</v>
       </c>
     </row>
@@ -11432,19 +11563,19 @@
         <v>2020</v>
       </c>
       <c r="B4" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4498995.0366637995</v>
       </c>
       <c r="C4" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>948290.90820388054</v>
       </c>
       <c r="D4" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5553490.0361212343</v>
       </c>
       <c r="E4" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2360108.8103560968</v>
       </c>
       <c r="F4" s="4">
@@ -11454,23 +11585,23 @@
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5655669.9322789013</v>
       </c>
       <c r="I4" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3669630.1536549246</v>
       </c>
       <c r="J4" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1999173.9889062068</v>
       </c>
       <c r="K4" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640133.73800439923</v>
       </c>
       <c r="L4" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640133.73800439923</v>
       </c>
       <c r="M4" s="4">
@@ -11489,7 +11620,7 @@
         <v>640133.73800439923</v>
       </c>
       <c r="Q4" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1392206.1767155745</v>
       </c>
     </row>
@@ -11498,19 +11629,19 @@
         <v>2021</v>
       </c>
       <c r="B5" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4469702.7155517321</v>
       </c>
       <c r="C5" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>941407.21093850711</v>
       </c>
       <c r="D5" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5513764.7148283115</v>
       </c>
       <c r="E5" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2323046.4138081288</v>
       </c>
       <c r="F5" s="4">
@@ -11520,23 +11651,23 @@
         <v>0</v>
       </c>
       <c r="H5" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5388387.243038536</v>
       </c>
       <c r="I5" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3710615.5803474663</v>
       </c>
       <c r="J5" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1863351.9852082757</v>
       </c>
       <c r="K5" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>632438.28065955907</v>
       </c>
       <c r="L5" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>632438.28065955907</v>
       </c>
       <c r="M5" s="4">
@@ -11555,7 +11686,7 @@
         <v>632438.28065955907</v>
       </c>
       <c r="Q5" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1407755.4723686662</v>
       </c>
     </row>
@@ -11564,19 +11695,19 @@
         <v>2022</v>
       </c>
       <c r="B6" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4440410.3944396656</v>
       </c>
       <c r="C6" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>934523.51367313403</v>
       </c>
       <c r="D6" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5474039.3935353896</v>
       </c>
       <c r="E6" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2285984.0172601612</v>
       </c>
       <c r="F6" s="4">
@@ -11586,23 +11717,23 @@
         <v>0</v>
       </c>
       <c r="H6" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5072088.2342516193</v>
       </c>
       <c r="I6" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3615350.5806739321</v>
       </c>
       <c r="J6" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1727529.9815103451</v>
       </c>
       <c r="K6" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>627720.5347827893</v>
       </c>
       <c r="L6" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>627720.5347827893</v>
       </c>
       <c r="M6" s="4">
@@ -11621,7 +11752,7 @@
         <v>627720.5347827893</v>
       </c>
       <c r="Q6" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1371613.268545154</v>
       </c>
     </row>
@@ -11630,19 +11761,19 @@
         <v>2023</v>
       </c>
       <c r="B7" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4411118.0733275991</v>
       </c>
       <c r="C7" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>920364.18721302296</v>
       </c>
       <c r="D7" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5434314.0722424677</v>
       </c>
       <c r="E7" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2248921.6207121932</v>
       </c>
       <c r="F7" s="4">
@@ -11652,23 +11783,23 @@
         <v>0</v>
       </c>
       <c r="H7" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4800966.0721755233</v>
       </c>
       <c r="I7" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3597882.1504836255</v>
       </c>
       <c r="J7" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1591707.9778124143</v>
       </c>
       <c r="K7" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>615347.58558829164</v>
       </c>
       <c r="L7" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>615347.58558829164</v>
       </c>
       <c r="M7" s="4">
@@ -11687,7 +11818,7 @@
         <v>615347.58558829164</v>
       </c>
       <c r="Q7" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1364985.9913019019</v>
       </c>
     </row>
@@ -11696,19 +11827,19 @@
         <v>2024</v>
       </c>
       <c r="B8" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4383925.9595025899</v>
       </c>
       <c r="C8" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>913239.77853647328</v>
       </c>
       <c r="D8" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5397190.1458511474</v>
       </c>
       <c r="E8" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2211859.2241642252</v>
       </c>
       <c r="F8" s="4">
@@ -11718,23 +11849,23 @@
         <v>0</v>
       </c>
       <c r="H8" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4505191.5170499301</v>
       </c>
       <c r="I8" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3582018.7353398106</v>
       </c>
       <c r="J8" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1455885.9741144832</v>
       </c>
       <c r="K8" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>609623.64132841176</v>
       </c>
       <c r="L8" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>609623.64132841176</v>
       </c>
       <c r="M8" s="4">
@@ -11753,7 +11884,7 @@
         <v>609623.64132841176</v>
       </c>
       <c r="Q8" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1358967.6342407612</v>
       </c>
     </row>
@@ -11762,19 +11893,19 @@
         <v>2025</v>
       </c>
       <c r="B9" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4374794.2380069029</v>
       </c>
       <c r="C9" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>909682.87820068328</v>
       </c>
       <c r="D9" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5382297.3522425154</v>
       </c>
       <c r="E9" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2174796.8276162585</v>
       </c>
       <c r="F9" s="4">
@@ -11784,23 +11915,23 @@
         <v>0</v>
       </c>
       <c r="H9" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4209416.9619243396</v>
       </c>
       <c r="I9" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3580152.8276873408</v>
       </c>
       <c r="J9" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1320063.9704165517</v>
       </c>
       <c r="K9" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>606223.36556319764</v>
       </c>
       <c r="L9" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>606223.36556319764</v>
       </c>
       <c r="M9" s="4">
@@ -11819,7 +11950,7 @@
         <v>606223.36556319764</v>
       </c>
       <c r="Q9" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1358259.7350655918</v>
       </c>
     </row>
@@ -11828,19 +11959,19 @@
         <v>2026</v>
       </c>
       <c r="B10" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4363916.1409849636</v>
       </c>
       <c r="C10" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>906052.87835925608</v>
       </c>
       <c r="D10" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5365239.2925965758</v>
       </c>
       <c r="E10" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2137734.4310682896</v>
       </c>
       <c r="F10" s="4">
@@ -11850,23 +11981,23 @@
         <v>0</v>
       </c>
       <c r="H10" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3913642.4067987497</v>
       </c>
       <c r="I10" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3576955.0329132001</v>
       </c>
       <c r="J10" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1184241.9667186209</v>
       </c>
       <c r="K10" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>602857.9705520398</v>
       </c>
       <c r="L10" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>602857.9705520398</v>
       </c>
       <c r="M10" s="4">
@@ -11885,7 +12016,7 @@
         <v>602857.9705520398</v>
       </c>
       <c r="Q10" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1357046.5366096133</v>
       </c>
     </row>
@@ -11894,19 +12025,19 @@
         <v>2027</v>
       </c>
       <c r="B11" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4350740.1611245479</v>
       </c>
       <c r="C11" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>902226.95651656261</v>
       </c>
       <c r="D11" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5345342.686611332</v>
       </c>
       <c r="E11" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2100672.0345203225</v>
       </c>
       <c r="F11" s="4">
@@ -11916,23 +12047,23 @@
         <v>0</v>
       </c>
       <c r="H11" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3617867.851673157</v>
       </c>
       <c r="I11" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3571990.797706374</v>
       </c>
       <c r="J11" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1048419.9630206898</v>
       </c>
       <c r="K11" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>599443.93548026006</v>
       </c>
       <c r="L11" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>599443.93548026006</v>
       </c>
       <c r="M11" s="4">
@@ -11951,7 +12082,7 @@
         <v>599443.93548026006</v>
       </c>
       <c r="Q11" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1355163.17544562</v>
       </c>
     </row>
@@ -11960,19 +12091,19 @@
         <v>2028</v>
       </c>
       <c r="B12" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4333046.343578591</v>
       </c>
       <c r="C12" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>898953.47467168875</v>
       </c>
       <c r="D12" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5319888.5323113659</v>
       </c>
       <c r="E12" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2063609.6379723544</v>
       </c>
       <c r="F12" s="4">
@@ -11982,23 +12113,23 @@
         <v>0</v>
       </c>
       <c r="H12" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3322093.2965475647</v>
       </c>
       <c r="I12" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3563521.302166706</v>
       </c>
       <c r="J12" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>912597.95932275837</v>
       </c>
       <c r="K12" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>596840.94162942353</v>
       </c>
       <c r="L12" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>596840.94162942353</v>
       </c>
       <c r="M12" s="4">
@@ -12017,7 +12148,7 @@
         <v>596840.94162942353</v>
       </c>
       <c r="Q12" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1351949.9677079825</v>
       </c>
     </row>
@@ -12026,19 +12157,19 @@
         <v>2029</v>
       </c>
       <c r="B13" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4306382.493295013</v>
       </c>
       <c r="C13" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>893843.22195435094</v>
       </c>
       <c r="D13" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5283424.9334751861</v>
       </c>
       <c r="E13" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2026547.2414243866</v>
       </c>
       <c r="F13" s="4">
@@ -12048,23 +12179,23 @@
         <v>0</v>
       </c>
       <c r="H13" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3026318.7414219733</v>
       </c>
       <c r="I13" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3548052.8540223199</v>
       </c>
       <c r="J13" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>776775.95562482707</v>
       </c>
       <c r="K13" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>593026.04321209737</v>
       </c>
       <c r="L13" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>593026.04321209737</v>
       </c>
       <c r="M13" s="4">
@@ -12083,7 +12214,7 @@
         <v>593026.04321209737</v>
       </c>
       <c r="Q13" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1346081.4555830292</v>
       </c>
     </row>
@@ -12092,19 +12223,19 @@
         <v>2030</v>
       </c>
       <c r="B14" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4286729.8869220419</v>
       </c>
       <c r="C14" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>890943.31681565102</v>
       </c>
       <c r="D14" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5255568.7933839113</v>
       </c>
       <c r="E14" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1989484.8448764191</v>
       </c>
       <c r="F14" s="4">
@@ -12114,23 +12245,23 @@
         <v>0</v>
       </c>
       <c r="H14" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2730544.1862963829</v>
       </c>
       <c r="I14" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3538051.4974978026</v>
       </c>
       <c r="J14" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K14" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>590905.00508873118</v>
       </c>
       <c r="L14" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>590905.00508873118</v>
       </c>
       <c r="M14" s="4">
@@ -12149,7 +12280,7 @@
         <v>590905.00508873118</v>
       </c>
       <c r="Q14" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1342287.0812875433</v>
       </c>
     </row>
@@ -12158,19 +12289,19 @@
         <v>2031</v>
       </c>
       <c r="B15" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4267192.1028447589</v>
       </c>
       <c r="C15" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>888253.39499304548</v>
       </c>
       <c r="D15" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5227852.1119602192</v>
       </c>
       <c r="E15" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1952422.4483284515</v>
       </c>
       <c r="F15" s="4">
@@ -12180,23 +12311,23 @@
         <v>0</v>
       </c>
       <c r="H15" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2703391.9892602018</v>
       </c>
       <c r="I15" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3528140.5335337119</v>
       </c>
       <c r="J15" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K15" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>588978.90673516935</v>
       </c>
       <c r="L15" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>588978.90673516935</v>
       </c>
       <c r="M15" s="4">
@@ -12215,7 +12346,7 @@
         <v>588978.90673516935</v>
       </c>
       <c r="Q15" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1338527.000660816</v>
       </c>
     </row>
@@ -12224,19 +12355,19 @@
         <v>2032</v>
       </c>
       <c r="B16" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4245321.0464447401</v>
       </c>
       <c r="C16" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>884611.0362725812</v>
       </c>
       <c r="D16" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5197278.1237860257</v>
       </c>
       <c r="E16" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1915360.0517804835</v>
       </c>
       <c r="F16" s="4">
@@ -12246,23 +12377,23 @@
         <v>0</v>
       </c>
       <c r="H16" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2676239.7922240188</v>
       </c>
       <c r="I16" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3516399.9480102807</v>
       </c>
       <c r="J16" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K16" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>586281.43813565525</v>
       </c>
       <c r="L16" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>586281.43813565525</v>
       </c>
       <c r="M16" s="4">
@@ -12281,7 +12412,7 @@
         <v>586281.43813565525</v>
       </c>
       <c r="Q16" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1334072.7872933741</v>
       </c>
     </row>
@@ -12290,19 +12421,19 @@
         <v>2033</v>
       </c>
       <c r="B17" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4225231.4989490611</v>
       </c>
       <c r="C17" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>881747.42832570034</v>
       </c>
       <c r="D17" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5168887.3612113139</v>
       </c>
       <c r="E17" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1878297.6552325157</v>
       </c>
       <c r="F17" s="4">
@@ -12312,23 +12443,23 @@
         <v>0</v>
       </c>
       <c r="H17" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2649087.5951878377</v>
       </c>
       <c r="I17" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3506054.8292013253</v>
       </c>
       <c r="J17" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K17" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>584222.64240803325</v>
       </c>
       <c r="L17" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>584222.64240803325</v>
       </c>
       <c r="M17" s="4">
@@ -12347,7 +12478,7 @@
         <v>584222.64240803325</v>
       </c>
       <c r="Q17" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1330147.9944119062</v>
       </c>
     </row>
@@ -12356,19 +12487,19 @@
         <v>2034</v>
       </c>
       <c r="B18" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4208463.5409309175</v>
       </c>
       <c r="C18" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>879278.49019149749</v>
       </c>
       <c r="D18" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5144556.9924184158</v>
       </c>
       <c r="E18" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1841235.2586845479</v>
       </c>
       <c r="F18" s="4">
@@ -12378,23 +12509,23 @@
         <v>0</v>
       </c>
       <c r="H18" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2621935.3981516548</v>
       </c>
       <c r="I18" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3498324.1015467704</v>
       </c>
       <c r="J18" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K18" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>582335.32315713551</v>
       </c>
       <c r="L18" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>582335.32315713551</v>
       </c>
       <c r="M18" s="4">
@@ -12413,7 +12544,7 @@
         <v>582335.32315713551</v>
       </c>
       <c r="Q18" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1327215.064841209</v>
       </c>
     </row>
@@ -12422,19 +12553,19 @@
         <v>2035</v>
       </c>
       <c r="B19" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4186398.8306184118</v>
       </c>
       <c r="C19" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>876080.77976725693</v>
       </c>
       <c r="D19" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5113751.0211141268</v>
       </c>
       <c r="E19" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1804172.86213658</v>
       </c>
       <c r="F19" s="4">
@@ -12444,23 +12575,23 @@
         <v>0</v>
       </c>
       <c r="H19" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2594783.2011154736</v>
       </c>
       <c r="I19" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3486425.1131533994</v>
       </c>
       <c r="J19" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K19" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>580078.88935867744</v>
       </c>
       <c r="L19" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>580078.88935867744</v>
       </c>
       <c r="M19" s="4">
@@ -12479,7 +12610,7 @@
         <v>580078.88935867744</v>
       </c>
       <c r="Q19" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1322700.7556481098</v>
       </c>
     </row>
@@ -12488,19 +12619,19 @@
         <v>2036</v>
       </c>
       <c r="B20" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4166126.8892237116</v>
       </c>
       <c r="C20" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>873031.18542034749</v>
       </c>
       <c r="D20" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5085136.6985640414</v>
       </c>
       <c r="E20" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1794462.9361779527</v>
       </c>
       <c r="F20" s="4">
@@ -12510,23 +12641,23 @@
         <v>0</v>
       </c>
       <c r="H20" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2567631.0040792916</v>
       </c>
       <c r="I20" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3475936.55756051</v>
       </c>
       <c r="J20" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K20" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>577852.50109153183</v>
       </c>
       <c r="L20" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>577852.50109153183</v>
       </c>
       <c r="M20" s="4">
@@ -12545,7 +12676,7 @@
         <v>577852.50109153183</v>
       </c>
       <c r="Q20" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1318721.5448639654</v>
       </c>
     </row>
@@ -12554,19 +12685,19 @@
         <v>2037</v>
       </c>
       <c r="B21" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4144856.7230918976</v>
       </c>
       <c r="C21" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>870245.50664545642</v>
       </c>
       <c r="D21" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5055305.8897382952</v>
       </c>
       <c r="E21" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1784753.010219326</v>
       </c>
       <c r="F21" s="4">
@@ -12576,23 +12707,23 @@
         <v>0</v>
       </c>
       <c r="H21" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2540478.80704311</v>
       </c>
       <c r="I21" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3464657.6933189998</v>
       </c>
       <c r="J21" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K21" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>575943.52100203745</v>
       </c>
       <c r="L21" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>575943.52100203745</v>
       </c>
       <c r="M21" s="4">
@@ -12611,7 +12742,7 @@
         <v>575943.52100203745</v>
       </c>
       <c r="Q21" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1314442.5020705855</v>
       </c>
     </row>
@@ -12620,19 +12751,19 @@
         <v>2038</v>
       </c>
       <c r="B22" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4125867.4823163347</v>
       </c>
       <c r="C22" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>868389.37121165253</v>
       </c>
       <c r="D22" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>5028258.59327613</v>
       </c>
       <c r="E22" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1775043.0842606986</v>
       </c>
       <c r="F22" s="4">
@@ -12642,23 +12773,23 @@
         <v>0</v>
       </c>
       <c r="H22" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2513326.610006928</v>
       </c>
       <c r="I22" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3455183.6645810818</v>
       </c>
       <c r="J22" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K22" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>574785.58623469959</v>
       </c>
       <c r="L22" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>574785.58623469959</v>
       </c>
       <c r="M22" s="4">
@@ -12677,7 +12808,7 @@
         <v>574785.58623469959</v>
       </c>
       <c r="Q22" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1310848.1885362437</v>
       </c>
     </row>
@@ -12686,19 +12817,19 @@
         <v>2039</v>
       </c>
       <c r="B23" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4104680.723820759</v>
       </c>
       <c r="C23" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>866070.37401335512</v>
       </c>
       <c r="D23" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4998531.5290436288</v>
       </c>
       <c r="E23" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1765333.158302071</v>
       </c>
       <c r="F23" s="4">
@@ -12708,23 +12839,23 @@
         <v>0</v>
       </c>
       <c r="H23" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2486174.4129707455</v>
       </c>
       <c r="I23" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3443966.4121572562</v>
       </c>
       <c r="J23" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K23" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>573321.26147515886</v>
       </c>
       <c r="L23" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>573321.26147515886</v>
       </c>
       <c r="M23" s="4">
@@ -12743,7 +12874,7 @@
         <v>573321.26147515886</v>
       </c>
       <c r="Q23" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1306592.5204017661</v>
       </c>
     </row>
@@ -12752,19 +12883,19 @@
         <v>2040</v>
       </c>
       <c r="B24" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4084014.7285643537</v>
       </c>
       <c r="C24" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>863860.25524858502</v>
       </c>
       <c r="D24" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4969440.6376708252</v>
       </c>
       <c r="E24" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1755623.2323434441</v>
       </c>
       <c r="F24" s="4">
@@ -12774,23 +12905,23 @@
         <v>0</v>
       </c>
       <c r="H24" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2459022.2159345644</v>
       </c>
       <c r="I24" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3433160.4520611921</v>
       </c>
       <c r="J24" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K24" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>571929.01977696037</v>
       </c>
       <c r="L24" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>571929.01977696037</v>
       </c>
       <c r="M24" s="4">
@@ -12809,7 +12940,7 @@
         <v>571929.01977696037</v>
       </c>
       <c r="Q24" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1302492.8908039173</v>
       </c>
     </row>
@@ -12818,19 +12949,19 @@
         <v>2041</v>
       </c>
       <c r="B25" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4067550.5033159018</v>
       </c>
       <c r="C25" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>862540.48501902213</v>
       </c>
       <c r="D25" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4945459.5905335443</v>
       </c>
       <c r="E25" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1745913.3063848168</v>
       </c>
       <c r="F25" s="4">
@@ -12840,23 +12971,23 @@
         <v>0</v>
       </c>
       <c r="H25" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2431870.0188983819</v>
       </c>
       <c r="I25" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3425700.1078922306</v>
       </c>
       <c r="J25" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K25" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>571126.25277404871</v>
       </c>
       <c r="L25" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>571126.25277404871</v>
       </c>
       <c r="M25" s="4">
@@ -12875,7 +13006,7 @@
         <v>571126.25277404871</v>
       </c>
       <c r="Q25" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1299662.5409327983</v>
       </c>
     </row>
@@ -12884,19 +13015,19 @@
         <v>2042</v>
       </c>
       <c r="B26" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4041919.4833016312</v>
       </c>
       <c r="C26" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>859275.63459266303</v>
       </c>
       <c r="D26" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4910336.3730173539</v>
       </c>
       <c r="E26" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1736203.3804261896</v>
       </c>
       <c r="F26" s="4">
@@ -12906,23 +13037,23 @@
         <v>0</v>
       </c>
       <c r="H26" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2404717.8218621998</v>
       </c>
       <c r="I26" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3410933.8741836962</v>
       </c>
       <c r="J26" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K26" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>569035.57651885482</v>
       </c>
       <c r="L26" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>569035.57651885482</v>
       </c>
       <c r="M26" s="4">
@@ -12941,7 +13072,7 @@
         <v>569035.57651885482</v>
       </c>
       <c r="Q26" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1294060.4391091652</v>
       </c>
     </row>
@@ -12950,19 +13081,19 @@
         <v>2043</v>
       </c>
       <c r="B27" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4027549.0846800846</v>
       </c>
       <c r="C27" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>858404.68064265454</v>
       </c>
       <c r="D27" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4888892.5746857012</v>
       </c>
       <c r="E27" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1726493.454467562</v>
       </c>
       <c r="F27" s="4">
@@ -12972,23 +13103,23 @@
         <v>0</v>
       </c>
       <c r="H27" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2377565.6248260182</v>
       </c>
       <c r="I27" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3405154.6476856545</v>
       </c>
       <c r="J27" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K27" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>568530.177953306</v>
       </c>
       <c r="L27" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>568530.177953306</v>
       </c>
       <c r="M27" s="4">
@@ -13007,7 +13138,7 @@
         <v>568530.177953306</v>
       </c>
       <c r="Q27" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1291867.8816877592</v>
       </c>
     </row>
@@ -13016,19 +13147,19 @@
         <v>2044</v>
       </c>
       <c r="B28" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>4002808.235279711</v>
       </c>
       <c r="C28" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>855323.90187924227</v>
       </c>
       <c r="D28" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4854859.1300343601</v>
       </c>
       <c r="E28" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1716783.5285089349</v>
       </c>
       <c r="F28" s="4">
@@ -13038,23 +13169,23 @@
         <v>0</v>
       </c>
       <c r="H28" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2350413.4277898367</v>
       </c>
       <c r="I28" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3391084.6066551027</v>
       </c>
       <c r="J28" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K28" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>566561.19400174171</v>
       </c>
       <c r="L28" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>566561.19400174171</v>
       </c>
       <c r="M28" s="4">
@@ -13073,7 +13204,7 @@
         <v>566561.19400174171</v>
       </c>
       <c r="Q28" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1286529.9055950278</v>
       </c>
     </row>
@@ -13082,19 +13213,19 @@
         <v>2045</v>
       </c>
       <c r="B29" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>3987525.789950409</v>
       </c>
       <c r="C29" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>854264.07546210196</v>
       </c>
       <c r="D29" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4832297.6878896719</v>
       </c>
       <c r="E29" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1707073.6025503075</v>
       </c>
       <c r="F29" s="4">
@@ -13104,23 +13235,23 @@
         <v>0</v>
       </c>
       <c r="H29" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2323261.2307536541</v>
       </c>
       <c r="I29" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3384590.2237373139</v>
       </c>
       <c r="J29" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K29" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>565930.83880835248</v>
       </c>
       <c r="L29" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>565930.83880835248</v>
       </c>
       <c r="M29" s="4">
@@ -13139,7 +13270,7 @@
         <v>565930.83880835248</v>
       </c>
       <c r="Q29" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1284066.0278652529</v>
       </c>
     </row>
@@ -13148,19 +13279,19 @@
         <v>2046</v>
       </c>
       <c r="B30" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>3964365.0723133213</v>
       </c>
       <c r="C30" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>851517.47797442612</v>
       </c>
       <c r="D30" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4800188.8840519451</v>
       </c>
       <c r="E30" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1697363.6765916804</v>
       </c>
       <c r="F30" s="4">
@@ -13170,23 +13301,23 @@
         <v>0</v>
       </c>
       <c r="H30" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2296109.0337174726</v>
       </c>
       <c r="I30" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3371777.3022148283</v>
       </c>
       <c r="J30" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K30" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>564183.11255323095</v>
       </c>
       <c r="L30" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>564183.11255323095</v>
       </c>
       <c r="M30" s="4">
@@ -13205,7 +13336,7 @@
         <v>564183.11255323095</v>
       </c>
       <c r="Q30" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1279204.9852700992</v>
       </c>
     </row>
@@ -13214,19 +13345,19 @@
         <v>2047</v>
       </c>
       <c r="B31" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>3944904.6700286916</v>
       </c>
       <c r="C31" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>849564.13218949281</v>
       </c>
       <c r="D31" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4772563.1483514039</v>
       </c>
       <c r="E31" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1687653.7506330532</v>
       </c>
       <c r="F31" s="4">
@@ -13236,23 +13367,23 @@
         <v>0</v>
       </c>
       <c r="H31" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2268956.8366812905</v>
       </c>
       <c r="I31" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3361934.7756505935</v>
       </c>
       <c r="J31" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K31" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>562960.8983085549</v>
       </c>
       <c r="L31" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>562960.8983085549</v>
       </c>
       <c r="M31" s="4">
@@ -13271,7 +13402,7 @@
         <v>562960.8983085549</v>
       </c>
       <c r="Q31" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1275470.8688323523</v>
       </c>
     </row>
@@ -13280,19 +13411,19 @@
         <v>2048</v>
       </c>
       <c r="B32" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>3925379.2073251978</v>
       </c>
       <c r="C32" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>847597.09481380892</v>
       </c>
       <c r="D32" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4744855.6043133195</v>
       </c>
       <c r="E32" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1677943.8246744261</v>
       </c>
       <c r="F32" s="4">
@@ -13302,23 +13433,23 @@
         <v>0</v>
       </c>
       <c r="H32" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2241804.6396451085</v>
       </c>
       <c r="I32" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3352040.6597777726</v>
       </c>
       <c r="J32" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K32" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>561729.66530371504</v>
       </c>
       <c r="L32" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>561729.66530371504</v>
       </c>
       <c r="M32" s="4">
@@ -13337,7 +13468,7 @@
         <v>561729.66530371504</v>
       </c>
       <c r="Q32" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1271717.1801349882</v>
       </c>
     </row>
@@ -13346,19 +13477,19 @@
         <v>2049</v>
       </c>
       <c r="B33" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>3905501.7363179387</v>
       </c>
       <c r="C33" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>845554.54963951895</v>
       </c>
       <c r="D33" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4716723.1390827727</v>
       </c>
       <c r="E33" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1668233.898715799</v>
       </c>
       <c r="F33" s="4">
@@ -13368,23 +13499,23 @@
         <v>0</v>
       </c>
       <c r="H33" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2214652.4426089264</v>
       </c>
       <c r="I33" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3341863.5705453139</v>
       </c>
       <c r="J33" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K33" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>560448.29901305423</v>
       </c>
       <c r="L33" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>560448.29901305423</v>
       </c>
       <c r="M33" s="4">
@@ -13403,7 +13534,7 @@
         <v>560448.29901305423</v>
       </c>
       <c r="Q33" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1267856.1353165335</v>
       </c>
     </row>
@@ -13412,19 +13543,19 @@
         <v>2050</v>
       </c>
       <c r="B34" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$61</f>
+        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
         <v>3855675.0986996656</v>
       </c>
       <c r="C34" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>837010.54636717902</v>
       </c>
       <c r="D34" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>4652452.4766705297</v>
       </c>
       <c r="E34" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1658523.9727571718</v>
       </c>
       <c r="F34" s="4">
@@ -13434,23 +13565,23 @@
         <v>0</v>
       </c>
       <c r="H34" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>2187500.2455727453</v>
       </c>
       <c r="I34" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>3307435.7945322236</v>
       </c>
       <c r="J34" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>640953.95192689588</v>
       </c>
       <c r="K34" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>554857.17842271458</v>
       </c>
       <c r="L34" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>554857.17842271458</v>
       </c>
       <c r="M34" s="4">
@@ -13469,7 +13600,7 @@
         <v>554857.17842271458</v>
       </c>
       <c r="Q34" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$65</f>
+        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
         <v>1254794.7202940234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Advance first simulated year from 2018 to 2019
</commit_message>
<xml_diff>
--- a/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
+++ b/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\elec\CCaMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D5C391-9B6B-41D8-9947-7A9F2F8329BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8719D44E-4CCC-476D-A9D2-38E83270BD0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="225" windowWidth="25050" windowHeight="16770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="825" windowWidth="24765" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -1740,6 +1740,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1763,12 +1769,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="228">
@@ -2689,10 +2689,10 @@
       <c r="K35" s="11"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="72" t="s">
+      <c r="A36" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="B36" s="73"/>
+      <c r="B36" s="65"/>
       <c r="D36" s="7"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -2703,10 +2703,10 @@
       <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="72" t="s">
+      <c r="A37" s="64" t="s">
         <v>234</v>
       </c>
-      <c r="B37" s="73"/>
+      <c r="B37" s="65"/>
       <c r="D37" s="7"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -4018,25 +4018,25 @@
       <c r="A2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="66" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4044,13 +4044,13 @@
       <c r="A3" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="65"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="67"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="27" t="s">
@@ -11347,7 +11347,7 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11425,92 +11425,92 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B2" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4557579.6788879326</v>
+        <v>4528287.3577758651</v>
       </c>
       <c r="C2" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>962058.30273462704</v>
+        <v>955174.60546925361</v>
       </c>
       <c r="D2" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5632940.678707079</v>
+        <v>5593215.3574141553</v>
       </c>
       <c r="E2" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2434233.6034520324</v>
+        <v>2397171.2069040639</v>
       </c>
       <c r="F2" s="20">
-        <f>'Start Year Wind and Solar'!B3*10^3*About!$A$71</f>
+        <f>'Start Year Wind and Solar'!$B$3*10^3*About!$A$71</f>
         <v>1344021</v>
       </c>
       <c r="G2" s="20">
-        <f>'Start Year Wind and Solar'!B7*10^6/About!$C$25*About!$A$71</f>
+        <f>'Start Year Wind and Solar'!$B$7*10^6/About!$C$25*About!$A$71</f>
         <v>1166557.3923166473</v>
       </c>
       <c r="H2" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>6190235.3107596356</v>
+        <v>5922952.6215192685</v>
       </c>
       <c r="I2" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3680479.6131787207</v>
+        <v>3675567.2263574409</v>
       </c>
       <c r="J2" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2270817.9963020692</v>
+        <v>2134995.9926041379</v>
       </c>
       <c r="K2" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>636580.52455604961</v>
+        <v>635581.04911209899</v>
       </c>
       <c r="L2" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>636580.52455604961</v>
+        <v>635581.04911209899</v>
       </c>
       <c r="M2" s="4">
         <f>B2*'Coal Cost Multipliers'!$B$33</f>
-        <v>5281971.7859389298</v>
+        <v>5248023.67651249</v>
       </c>
       <c r="N2" s="20">
-        <f>SUMPRODUCT('Cost Improvement and Off Wnd'!B45:B59,'Cost Improvement and Off Wnd'!C27:C41)/SUM('Cost Improvement and Off Wnd'!B45:B59)*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("offshore wind",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH(A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*10^3*About!$A$71</f>
-        <v>3030248.6826914768</v>
+        <f>SUMPRODUCT('Cost Improvement and Off Wnd'!B46:B60,'Cost Improvement and Off Wnd'!C28:C42)/SUM('Cost Improvement and Off Wnd'!B46:B60)*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("offshore wind",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH(A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*10^3*About!$A$71</f>
+        <v>2918095.5206037629</v>
       </c>
       <c r="O2" s="4">
-        <f>K2</f>
-        <v>636580.52455604961</v>
+        <f t="shared" ref="O2:O33" si="0">K2</f>
+        <v>635581.04911209899</v>
       </c>
       <c r="P2" s="4">
-        <f>K2</f>
-        <v>636580.52455604961</v>
+        <f t="shared" ref="P2:P33" si="1">K2</f>
+        <v>635581.04911209899</v>
       </c>
       <c r="Q2" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A2,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1396322.3093857865</v>
+        <v>1394458.6187715731</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B3" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4528287.3577758651</v>
+        <v>4498995.0366637995</v>
       </c>
       <c r="C3" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>955174.60546925361</v>
+        <v>948290.90820388054</v>
       </c>
       <c r="D3" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5593215.3574141553</v>
+        <v>5553490.0361212343</v>
       </c>
       <c r="E3" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2397171.2069040639</v>
+        <v>2360108.8103560968</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
@@ -11520,63 +11520,63 @@
       </c>
       <c r="H3" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5922952.6215192685</v>
+        <v>5655669.9322789013</v>
       </c>
       <c r="I3" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3675567.2263574409</v>
+        <v>3669630.1536549246</v>
       </c>
       <c r="J3" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2134995.9926041379</v>
+        <v>1999173.9889062068</v>
       </c>
       <c r="K3" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>635581.04911209899</v>
+        <v>640133.73800439923</v>
       </c>
       <c r="L3" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>635581.04911209899</v>
+        <v>640133.73800439923</v>
       </c>
       <c r="M3" s="4">
         <f>B3*'Coal Cost Multipliers'!$B$33</f>
-        <v>5248023.67651249</v>
+        <v>5214075.5670860531</v>
       </c>
       <c r="N3" s="4">
         <v>0</v>
       </c>
       <c r="O3" s="4">
-        <f t="shared" ref="O3:O34" si="0">K3</f>
-        <v>635581.04911209899</v>
+        <f t="shared" si="0"/>
+        <v>640133.73800439923</v>
       </c>
       <c r="P3" s="4">
-        <f t="shared" ref="P3:P34" si="1">K3</f>
-        <v>635581.04911209899</v>
+        <f t="shared" si="1"/>
+        <v>640133.73800439923</v>
       </c>
       <c r="Q3" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A3,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1394458.6187715731</v>
+        <v>1392206.1767155745</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B4" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4498995.0366637995</v>
+        <v>4469702.7155517321</v>
       </c>
       <c r="C4" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>948290.90820388054</v>
+        <v>941407.21093850711</v>
       </c>
       <c r="D4" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5553490.0361212343</v>
+        <v>5513764.7148283115</v>
       </c>
       <c r="E4" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2360108.8103560968</v>
+        <v>2323046.4138081288</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -11586,63 +11586,63 @@
       </c>
       <c r="H4" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5655669.9322789013</v>
+        <v>5388387.243038536</v>
       </c>
       <c r="I4" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3669630.1536549246</v>
+        <v>3710615.5803474663</v>
       </c>
       <c r="J4" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1999173.9889062068</v>
+        <v>1863351.9852082757</v>
       </c>
       <c r="K4" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>640133.73800439923</v>
+        <v>632438.28065955907</v>
       </c>
       <c r="L4" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>640133.73800439923</v>
+        <v>632438.28065955907</v>
       </c>
       <c r="M4" s="4">
         <f>B4*'Coal Cost Multipliers'!$B$33</f>
-        <v>5214075.5670860531</v>
+        <v>5180127.4576596133</v>
       </c>
       <c r="N4" s="4">
         <v>0</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="0"/>
-        <v>640133.73800439923</v>
+        <v>632438.28065955907</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="1"/>
-        <v>640133.73800439923</v>
+        <v>632438.28065955907</v>
       </c>
       <c r="Q4" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A4,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1392206.1767155745</v>
+        <v>1407755.4723686662</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B5" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4469702.7155517321</v>
+        <v>4440410.3944396656</v>
       </c>
       <c r="C5" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>941407.21093850711</v>
+        <v>934523.51367313403</v>
       </c>
       <c r="D5" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5513764.7148283115</v>
+        <v>5474039.3935353896</v>
       </c>
       <c r="E5" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2323046.4138081288</v>
+        <v>2285984.0172601612</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
@@ -11652,63 +11652,63 @@
       </c>
       <c r="H5" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5388387.243038536</v>
+        <v>5072088.2342516193</v>
       </c>
       <c r="I5" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3710615.5803474663</v>
+        <v>3615350.5806739321</v>
       </c>
       <c r="J5" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1863351.9852082757</v>
+        <v>1727529.9815103451</v>
       </c>
       <c r="K5" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>632438.28065955907</v>
+        <v>627720.5347827893</v>
       </c>
       <c r="L5" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>632438.28065955907</v>
+        <v>627720.5347827893</v>
       </c>
       <c r="M5" s="4">
         <f>B5*'Coal Cost Multipliers'!$B$33</f>
-        <v>5180127.4576596133</v>
+        <v>5146179.3482331755</v>
       </c>
       <c r="N5" s="4">
         <v>0</v>
       </c>
       <c r="O5" s="4">
         <f t="shared" si="0"/>
-        <v>632438.28065955907</v>
+        <v>627720.5347827893</v>
       </c>
       <c r="P5" s="4">
         <f t="shared" si="1"/>
-        <v>632438.28065955907</v>
+        <v>627720.5347827893</v>
       </c>
       <c r="Q5" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A5,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1407755.4723686662</v>
+        <v>1371613.268545154</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B6" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4440410.3944396656</v>
+        <v>4411118.0733275991</v>
       </c>
       <c r="C6" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>934523.51367313403</v>
+        <v>920364.18721302296</v>
       </c>
       <c r="D6" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5474039.3935353896</v>
+        <v>5434314.0722424677</v>
       </c>
       <c r="E6" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2285984.0172601612</v>
+        <v>2248921.6207121932</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -11718,63 +11718,63 @@
       </c>
       <c r="H6" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5072088.2342516193</v>
+        <v>4800966.0721755233</v>
       </c>
       <c r="I6" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3615350.5806739321</v>
+        <v>3597882.1504836255</v>
       </c>
       <c r="J6" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1727529.9815103451</v>
+        <v>1591707.9778124143</v>
       </c>
       <c r="K6" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>627720.5347827893</v>
+        <v>615347.58558829164</v>
       </c>
       <c r="L6" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>627720.5347827893</v>
+        <v>615347.58558829164</v>
       </c>
       <c r="M6" s="4">
         <f>B6*'Coal Cost Multipliers'!$B$33</f>
-        <v>5146179.3482331755</v>
+        <v>5112231.2388067376</v>
       </c>
       <c r="N6" s="4">
         <v>0</v>
       </c>
       <c r="O6" s="4">
         <f t="shared" si="0"/>
-        <v>627720.5347827893</v>
+        <v>615347.58558829164</v>
       </c>
       <c r="P6" s="4">
         <f t="shared" si="1"/>
-        <v>627720.5347827893</v>
+        <v>615347.58558829164</v>
       </c>
       <c r="Q6" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A6,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1371613.268545154</v>
+        <v>1364985.9913019019</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B7" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4411118.0733275991</v>
+        <v>4383925.9595025899</v>
       </c>
       <c r="C7" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>920364.18721302296</v>
+        <v>913239.77853647328</v>
       </c>
       <c r="D7" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5434314.0722424677</v>
+        <v>5397190.1458511474</v>
       </c>
       <c r="E7" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2248921.6207121932</v>
+        <v>2211859.2241642252</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -11784,63 +11784,63 @@
       </c>
       <c r="H7" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4800966.0721755233</v>
+        <v>4505191.5170499301</v>
       </c>
       <c r="I7" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3597882.1504836255</v>
+        <v>3582018.7353398106</v>
       </c>
       <c r="J7" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1591707.9778124143</v>
+        <v>1455885.9741144832</v>
       </c>
       <c r="K7" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>615347.58558829164</v>
+        <v>609623.64132841176</v>
       </c>
       <c r="L7" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>615347.58558829164</v>
+        <v>609623.64132841176</v>
       </c>
       <c r="M7" s="4">
         <f>B7*'Coal Cost Multipliers'!$B$33</f>
-        <v>5112231.2388067376</v>
+        <v>5080717.1484027747</v>
       </c>
       <c r="N7" s="4">
         <v>0</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="0"/>
-        <v>615347.58558829164</v>
+        <v>609623.64132841176</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" si="1"/>
-        <v>615347.58558829164</v>
+        <v>609623.64132841176</v>
       </c>
       <c r="Q7" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A7,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1364985.9913019019</v>
+        <v>1358967.6342407612</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B8" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4383925.9595025899</v>
+        <v>4374794.2380069029</v>
       </c>
       <c r="C8" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>913239.77853647328</v>
+        <v>909682.87820068328</v>
       </c>
       <c r="D8" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5397190.1458511474</v>
+        <v>5382297.3522425154</v>
       </c>
       <c r="E8" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2211859.2241642252</v>
+        <v>2174796.8276162585</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -11850,63 +11850,63 @@
       </c>
       <c r="H8" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4505191.5170499301</v>
+        <v>4209416.9619243396</v>
       </c>
       <c r="I8" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3582018.7353398106</v>
+        <v>3580152.8276873408</v>
       </c>
       <c r="J8" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1455885.9741144832</v>
+        <v>1320063.9704165517</v>
       </c>
       <c r="K8" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>609623.64132841176</v>
+        <v>606223.36556319764</v>
       </c>
       <c r="L8" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>609623.64132841176</v>
+        <v>606223.36556319764</v>
       </c>
       <c r="M8" s="4">
         <f>B8*'Coal Cost Multipliers'!$B$33</f>
-        <v>5080717.1484027747</v>
+        <v>5070134.0102690179</v>
       </c>
       <c r="N8" s="4">
         <v>0</v>
       </c>
       <c r="O8" s="4">
         <f t="shared" si="0"/>
-        <v>609623.64132841176</v>
+        <v>606223.36556319764</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="1"/>
-        <v>609623.64132841176</v>
+        <v>606223.36556319764</v>
       </c>
       <c r="Q8" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A8,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1358967.6342407612</v>
+        <v>1358259.7350655918</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="1">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B9" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4374794.2380069029</v>
+        <v>4363916.1409849636</v>
       </c>
       <c r="C9" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>909682.87820068328</v>
+        <v>906052.87835925608</v>
       </c>
       <c r="D9" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5382297.3522425154</v>
+        <v>5365239.2925965758</v>
       </c>
       <c r="E9" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2174796.8276162585</v>
+        <v>2137734.4310682896</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -11916,63 +11916,63 @@
       </c>
       <c r="H9" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4209416.9619243396</v>
+        <v>3913642.4067987497</v>
       </c>
       <c r="I9" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3580152.8276873408</v>
+        <v>3576955.0329132001</v>
       </c>
       <c r="J9" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1320063.9704165517</v>
+        <v>1184241.9667186209</v>
       </c>
       <c r="K9" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>606223.36556319764</v>
+        <v>602857.9705520398</v>
       </c>
       <c r="L9" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>606223.36556319764</v>
+        <v>602857.9705520398</v>
       </c>
       <c r="M9" s="4">
         <f>B9*'Coal Cost Multipliers'!$B$33</f>
-        <v>5070134.0102690179</v>
+        <v>5057526.9237005152</v>
       </c>
       <c r="N9" s="4">
         <v>0</v>
       </c>
       <c r="O9" s="4">
         <f t="shared" si="0"/>
-        <v>606223.36556319764</v>
+        <v>602857.9705520398</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" si="1"/>
-        <v>606223.36556319764</v>
+        <v>602857.9705520398</v>
       </c>
       <c r="Q9" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A9,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1358259.7350655918</v>
+        <v>1357046.5366096133</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="1">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B10" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4363916.1409849636</v>
+        <v>4350740.1611245479</v>
       </c>
       <c r="C10" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>906052.87835925608</v>
+        <v>902226.95651656261</v>
       </c>
       <c r="D10" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5365239.2925965758</v>
+        <v>5345342.686611332</v>
       </c>
       <c r="E10" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2137734.4310682896</v>
+        <v>2100672.0345203225</v>
       </c>
       <c r="F10" s="4">
         <v>0</v>
@@ -11982,63 +11982,63 @@
       </c>
       <c r="H10" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3913642.4067987497</v>
+        <v>3617867.851673157</v>
       </c>
       <c r="I10" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3576955.0329132001</v>
+        <v>3571990.797706374</v>
       </c>
       <c r="J10" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1184241.9667186209</v>
+        <v>1048419.9630206898</v>
       </c>
       <c r="K10" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>602857.9705520398</v>
+        <v>599443.93548026006</v>
       </c>
       <c r="L10" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>602857.9705520398</v>
+        <v>599443.93548026006</v>
       </c>
       <c r="M10" s="4">
         <f>B10*'Coal Cost Multipliers'!$B$33</f>
-        <v>5057526.9237005152</v>
+        <v>5042256.7235552054</v>
       </c>
       <c r="N10" s="4">
         <v>0</v>
       </c>
       <c r="O10" s="4">
         <f t="shared" si="0"/>
-        <v>602857.9705520398</v>
+        <v>599443.93548026006</v>
       </c>
       <c r="P10" s="4">
         <f t="shared" si="1"/>
-        <v>602857.9705520398</v>
+        <v>599443.93548026006</v>
       </c>
       <c r="Q10" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A10,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1357046.5366096133</v>
+        <v>1355163.17544562</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="1">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B11" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4350740.1611245479</v>
+        <v>4333046.343578591</v>
       </c>
       <c r="C11" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>902226.95651656261</v>
+        <v>898953.47467168875</v>
       </c>
       <c r="D11" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5345342.686611332</v>
+        <v>5319888.5323113659</v>
       </c>
       <c r="E11" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2100672.0345203225</v>
+        <v>2063609.6379723544</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -12048,63 +12048,63 @@
       </c>
       <c r="H11" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3617867.851673157</v>
+        <v>3322093.2965475647</v>
       </c>
       <c r="I11" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3571990.797706374</v>
+        <v>3563521.302166706</v>
       </c>
       <c r="J11" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1048419.9630206898</v>
+        <v>912597.95932275837</v>
       </c>
       <c r="K11" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>599443.93548026006</v>
+        <v>596840.94162942353</v>
       </c>
       <c r="L11" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>599443.93548026006</v>
+        <v>596840.94162942353</v>
       </c>
       <c r="M11" s="4">
         <f>B11*'Coal Cost Multipliers'!$B$33</f>
-        <v>5042256.7235552054</v>
+        <v>5021750.6103003519</v>
       </c>
       <c r="N11" s="4">
         <v>0</v>
       </c>
       <c r="O11" s="4">
         <f t="shared" si="0"/>
-        <v>599443.93548026006</v>
+        <v>596840.94162942353</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" si="1"/>
-        <v>599443.93548026006</v>
+        <v>596840.94162942353</v>
       </c>
       <c r="Q11" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1355163.17544562</v>
+        <v>1351949.9677079825</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="1">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B12" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4333046.343578591</v>
+        <v>4306382.493295013</v>
       </c>
       <c r="C12" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>898953.47467168875</v>
+        <v>893843.22195435094</v>
       </c>
       <c r="D12" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5319888.5323113659</v>
+        <v>5283424.9334751861</v>
       </c>
       <c r="E12" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2063609.6379723544</v>
+        <v>2026547.2414243866</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -12114,63 +12114,63 @@
       </c>
       <c r="H12" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3322093.2965475647</v>
+        <v>3026318.7414219733</v>
       </c>
       <c r="I12" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3563521.302166706</v>
+        <v>3548052.8540223199</v>
       </c>
       <c r="J12" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>912597.95932275837</v>
+        <v>776775.95562482707</v>
       </c>
       <c r="K12" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>596840.94162942353</v>
+        <v>593026.04321209737</v>
       </c>
       <c r="L12" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>596840.94162942353</v>
+        <v>593026.04321209737</v>
       </c>
       <c r="M12" s="4">
         <f>B12*'Coal Cost Multipliers'!$B$33</f>
-        <v>5021750.6103003519</v>
+        <v>4990848.7468497222</v>
       </c>
       <c r="N12" s="4">
         <v>0</v>
       </c>
       <c r="O12" s="4">
         <f t="shared" si="0"/>
-        <v>596840.94162942353</v>
+        <v>593026.04321209737</v>
       </c>
       <c r="P12" s="4">
         <f t="shared" si="1"/>
-        <v>596840.94162942353</v>
+        <v>593026.04321209737</v>
       </c>
       <c r="Q12" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1351949.9677079825</v>
+        <v>1346081.4555830292</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B13" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4306382.493295013</v>
+        <v>4286729.8869220419</v>
       </c>
       <c r="C13" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>893843.22195435094</v>
+        <v>890943.31681565102</v>
       </c>
       <c r="D13" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5283424.9334751861</v>
+        <v>5255568.7933839113</v>
       </c>
       <c r="E13" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2026547.2414243866</v>
+        <v>1989484.8448764191</v>
       </c>
       <c r="F13" s="4">
         <v>0</v>
@@ -12180,63 +12180,63 @@
       </c>
       <c r="H13" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3026318.7414219733</v>
+        <v>2730544.1862963829</v>
       </c>
       <c r="I13" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3548052.8540223199</v>
+        <v>3538051.4974978026</v>
       </c>
       <c r="J13" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>776775.95562482707</v>
+        <v>640953.95192689588</v>
       </c>
       <c r="K13" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>593026.04321209737</v>
+        <v>590905.00508873118</v>
       </c>
       <c r="L13" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>593026.04321209737</v>
+        <v>590905.00508873118</v>
       </c>
       <c r="M13" s="4">
         <f>B13*'Coal Cost Multipliers'!$B$33</f>
-        <v>4990848.7468497222</v>
+        <v>4968072.5104049603</v>
       </c>
       <c r="N13" s="4">
         <v>0</v>
       </c>
       <c r="O13" s="4">
         <f t="shared" si="0"/>
-        <v>593026.04321209737</v>
+        <v>590905.00508873118</v>
       </c>
       <c r="P13" s="4">
         <f t="shared" si="1"/>
-        <v>593026.04321209737</v>
+        <v>590905.00508873118</v>
       </c>
       <c r="Q13" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1346081.4555830292</v>
+        <v>1342287.0812875433</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="1">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B14" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4286729.8869220419</v>
+        <v>4267192.1028447589</v>
       </c>
       <c r="C14" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>890943.31681565102</v>
+        <v>888253.39499304548</v>
       </c>
       <c r="D14" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5255568.7933839113</v>
+        <v>5227852.1119602192</v>
       </c>
       <c r="E14" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1989484.8448764191</v>
+        <v>1952422.4483284515</v>
       </c>
       <c r="F14" s="4">
         <v>0</v>
@@ -12246,11 +12246,11 @@
       </c>
       <c r="H14" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2730544.1862963829</v>
+        <v>2703391.9892602018</v>
       </c>
       <c r="I14" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3538051.4974978026</v>
+        <v>3528140.5335337119</v>
       </c>
       <c r="J14" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12258,51 +12258,51 @@
       </c>
       <c r="K14" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>590905.00508873118</v>
+        <v>588978.90673516935</v>
       </c>
       <c r="L14" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>590905.00508873118</v>
+        <v>588978.90673516935</v>
       </c>
       <c r="M14" s="4">
         <f>B14*'Coal Cost Multipliers'!$B$33</f>
-        <v>4968072.5104049603</v>
+        <v>4945429.3463733969</v>
       </c>
       <c r="N14" s="4">
         <v>0</v>
       </c>
       <c r="O14" s="4">
         <f t="shared" si="0"/>
-        <v>590905.00508873118</v>
+        <v>588978.90673516935</v>
       </c>
       <c r="P14" s="4">
         <f t="shared" si="1"/>
-        <v>590905.00508873118</v>
+        <v>588978.90673516935</v>
       </c>
       <c r="Q14" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1342287.0812875433</v>
+        <v>1338527.000660816</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B15" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4267192.1028447589</v>
+        <v>4245321.0464447401</v>
       </c>
       <c r="C15" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>888253.39499304548</v>
+        <v>884611.0362725812</v>
       </c>
       <c r="D15" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5227852.1119602192</v>
+        <v>5197278.1237860257</v>
       </c>
       <c r="E15" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1952422.4483284515</v>
+        <v>1915360.0517804835</v>
       </c>
       <c r="F15" s="4">
         <v>0</v>
@@ -12312,11 +12312,11 @@
       </c>
       <c r="H15" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2703391.9892602018</v>
+        <v>2676239.7922240188</v>
       </c>
       <c r="I15" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3528140.5335337119</v>
+        <v>3516399.9480102807</v>
       </c>
       <c r="J15" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12324,51 +12324,51 @@
       </c>
       <c r="K15" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>588978.90673516935</v>
+        <v>586281.43813565525</v>
       </c>
       <c r="L15" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>588978.90673516935</v>
+        <v>586281.43813565525</v>
       </c>
       <c r="M15" s="4">
         <f>B15*'Coal Cost Multipliers'!$B$33</f>
-        <v>4945429.3463733969</v>
+        <v>4920082.05439544</v>
       </c>
       <c r="N15" s="4">
         <v>0</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="0"/>
-        <v>588978.90673516935</v>
+        <v>586281.43813565525</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="1"/>
-        <v>588978.90673516935</v>
+        <v>586281.43813565525</v>
       </c>
       <c r="Q15" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1338527.000660816</v>
+        <v>1334072.7872933741</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="1">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B16" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4245321.0464447401</v>
+        <v>4225231.4989490611</v>
       </c>
       <c r="C16" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>884611.0362725812</v>
+        <v>881747.42832570034</v>
       </c>
       <c r="D16" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5197278.1237860257</v>
+        <v>5168887.3612113139</v>
       </c>
       <c r="E16" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1915360.0517804835</v>
+        <v>1878297.6552325157</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -12378,11 +12378,11 @@
       </c>
       <c r="H16" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2676239.7922240188</v>
+        <v>2649087.5951878377</v>
       </c>
       <c r="I16" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3516399.9480102807</v>
+        <v>3506054.8292013253</v>
       </c>
       <c r="J16" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12390,51 +12390,51 @@
       </c>
       <c r="K16" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>586281.43813565525</v>
+        <v>584222.64240803325</v>
       </c>
       <c r="L16" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>586281.43813565525</v>
+        <v>584222.64240803325</v>
       </c>
       <c r="M16" s="4">
         <f>B16*'Coal Cost Multipliers'!$B$33</f>
-        <v>4920082.05439544</v>
+        <v>4896799.4284095466</v>
       </c>
       <c r="N16" s="4">
         <v>0</v>
       </c>
       <c r="O16" s="4">
         <f t="shared" si="0"/>
-        <v>586281.43813565525</v>
+        <v>584222.64240803325</v>
       </c>
       <c r="P16" s="4">
         <f t="shared" si="1"/>
-        <v>586281.43813565525</v>
+        <v>584222.64240803325</v>
       </c>
       <c r="Q16" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1334072.7872933741</v>
+        <v>1330147.9944119062</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B17" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4225231.4989490611</v>
+        <v>4208463.5409309175</v>
       </c>
       <c r="C17" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>881747.42832570034</v>
+        <v>879278.49019149749</v>
       </c>
       <c r="D17" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5168887.3612113139</v>
+        <v>5144556.9924184158</v>
       </c>
       <c r="E17" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1878297.6552325157</v>
+        <v>1841235.2586845479</v>
       </c>
       <c r="F17" s="4">
         <v>0</v>
@@ -12444,11 +12444,11 @@
       </c>
       <c r="H17" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2649087.5951878377</v>
+        <v>2621935.3981516548</v>
       </c>
       <c r="I17" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3506054.8292013253</v>
+        <v>3498324.1015467704</v>
       </c>
       <c r="J17" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12456,51 +12456,51 @@
       </c>
       <c r="K17" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>584222.64240803325</v>
+        <v>582335.32315713551</v>
       </c>
       <c r="L17" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>584222.64240803325</v>
+        <v>582335.32315713551</v>
       </c>
       <c r="M17" s="4">
         <f>B17*'Coal Cost Multipliers'!$B$33</f>
-        <v>4896799.4284095466</v>
+        <v>4877366.332907143</v>
       </c>
       <c r="N17" s="4">
         <v>0</v>
       </c>
       <c r="O17" s="4">
         <f t="shared" si="0"/>
-        <v>584222.64240803325</v>
+        <v>582335.32315713551</v>
       </c>
       <c r="P17" s="4">
         <f t="shared" si="1"/>
-        <v>584222.64240803325</v>
+        <v>582335.32315713551</v>
       </c>
       <c r="Q17" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1330147.9944119062</v>
+        <v>1327215.064841209</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="1">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B18" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4208463.5409309175</v>
+        <v>4186398.8306184118</v>
       </c>
       <c r="C18" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>879278.49019149749</v>
+        <v>876080.77976725693</v>
       </c>
       <c r="D18" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5144556.9924184158</v>
+        <v>5113751.0211141268</v>
       </c>
       <c r="E18" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1841235.2586845479</v>
+        <v>1804172.86213658</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
@@ -12510,11 +12510,11 @@
       </c>
       <c r="H18" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2621935.3981516548</v>
+        <v>2594783.2011154736</v>
       </c>
       <c r="I18" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3498324.1015467704</v>
+        <v>3486425.1131533994</v>
       </c>
       <c r="J18" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12522,51 +12522,51 @@
       </c>
       <c r="K18" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>582335.32315713551</v>
+        <v>580078.88935867744</v>
       </c>
       <c r="L18" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>582335.32315713551</v>
+        <v>580078.88935867744</v>
       </c>
       <c r="M18" s="4">
         <f>B18*'Coal Cost Multipliers'!$B$33</f>
-        <v>4877366.332907143</v>
+        <v>4851794.6072222488</v>
       </c>
       <c r="N18" s="4">
         <v>0</v>
       </c>
       <c r="O18" s="4">
         <f t="shared" si="0"/>
-        <v>582335.32315713551</v>
+        <v>580078.88935867744</v>
       </c>
       <c r="P18" s="4">
         <f t="shared" si="1"/>
-        <v>582335.32315713551</v>
+        <v>580078.88935867744</v>
       </c>
       <c r="Q18" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1327215.064841209</v>
+        <v>1322700.7556481098</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="1">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B19" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4186398.8306184118</v>
+        <v>4166126.8892237116</v>
       </c>
       <c r="C19" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>876080.77976725693</v>
+        <v>873031.18542034749</v>
       </c>
       <c r="D19" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5113751.0211141268</v>
+        <v>5085136.6985640414</v>
       </c>
       <c r="E19" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1804172.86213658</v>
+        <v>1794462.9361779527</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -12576,11 +12576,11 @@
       </c>
       <c r="H19" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2594783.2011154736</v>
+        <v>2567631.0040792916</v>
       </c>
       <c r="I19" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3486425.1131533994</v>
+        <v>3475936.55756051</v>
       </c>
       <c r="J19" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12588,51 +12588,51 @@
       </c>
       <c r="K19" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>580078.88935867744</v>
+        <v>577852.50109153183</v>
       </c>
       <c r="L19" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>580078.88935867744</v>
+        <v>577852.50109153183</v>
       </c>
       <c r="M19" s="4">
         <f>B19*'Coal Cost Multipliers'!$B$33</f>
-        <v>4851794.6072222488</v>
+        <v>4828300.5972351003</v>
       </c>
       <c r="N19" s="4">
         <v>0</v>
       </c>
       <c r="O19" s="4">
         <f t="shared" si="0"/>
-        <v>580078.88935867744</v>
+        <v>577852.50109153183</v>
       </c>
       <c r="P19" s="4">
         <f t="shared" si="1"/>
-        <v>580078.88935867744</v>
+        <v>577852.50109153183</v>
       </c>
       <c r="Q19" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1322700.7556481098</v>
+        <v>1318721.5448639654</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="1">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B20" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4166126.8892237116</v>
+        <v>4144856.7230918976</v>
       </c>
       <c r="C20" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>873031.18542034749</v>
+        <v>870245.50664545642</v>
       </c>
       <c r="D20" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5085136.6985640414</v>
+        <v>5055305.8897382952</v>
       </c>
       <c r="E20" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1794462.9361779527</v>
+        <v>1784753.010219326</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -12642,11 +12642,11 @@
       </c>
       <c r="H20" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2567631.0040792916</v>
+        <v>2540478.80704311</v>
       </c>
       <c r="I20" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3475936.55756051</v>
+        <v>3464657.6933189998</v>
       </c>
       <c r="J20" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12654,51 +12654,51 @@
       </c>
       <c r="K20" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>577852.50109153183</v>
+        <v>575943.52100203745</v>
       </c>
       <c r="L20" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>577852.50109153183</v>
+        <v>575943.52100203745</v>
       </c>
       <c r="M20" s="4">
         <f>B20*'Coal Cost Multipliers'!$B$33</f>
-        <v>4828300.5972351003</v>
+        <v>4803649.702394818</v>
       </c>
       <c r="N20" s="4">
         <v>0</v>
       </c>
       <c r="O20" s="4">
         <f t="shared" si="0"/>
-        <v>577852.50109153183</v>
+        <v>575943.52100203745</v>
       </c>
       <c r="P20" s="4">
         <f t="shared" si="1"/>
-        <v>577852.50109153183</v>
+        <v>575943.52100203745</v>
       </c>
       <c r="Q20" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1318721.5448639654</v>
+        <v>1314442.5020705855</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="1">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B21" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4144856.7230918976</v>
+        <v>4125867.4823163347</v>
       </c>
       <c r="C21" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>870245.50664545642</v>
+        <v>868389.37121165253</v>
       </c>
       <c r="D21" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5055305.8897382952</v>
+        <v>5028258.59327613</v>
       </c>
       <c r="E21" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1784753.010219326</v>
+        <v>1775043.0842606986</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
@@ -12708,11 +12708,11 @@
       </c>
       <c r="H21" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2540478.80704311</v>
+        <v>2513326.610006928</v>
       </c>
       <c r="I21" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3464657.6933189998</v>
+        <v>3455183.6645810818</v>
       </c>
       <c r="J21" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12720,51 +12720,51 @@
       </c>
       <c r="K21" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>575943.52100203745</v>
+        <v>574785.58623469959</v>
       </c>
       <c r="L21" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>575943.52100203745</v>
+        <v>574785.58623469959</v>
       </c>
       <c r="M21" s="4">
         <f>B21*'Coal Cost Multipliers'!$B$33</f>
-        <v>4803649.702394818</v>
+        <v>4781642.2683882229</v>
       </c>
       <c r="N21" s="4">
         <v>0</v>
       </c>
       <c r="O21" s="4">
         <f t="shared" si="0"/>
-        <v>575943.52100203745</v>
+        <v>574785.58623469959</v>
       </c>
       <c r="P21" s="4">
         <f t="shared" si="1"/>
-        <v>575943.52100203745</v>
+        <v>574785.58623469959</v>
       </c>
       <c r="Q21" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1314442.5020705855</v>
+        <v>1310848.1885362437</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="1">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B22" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4125867.4823163347</v>
+        <v>4104680.723820759</v>
       </c>
       <c r="C22" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>868389.37121165253</v>
+        <v>866070.37401335512</v>
       </c>
       <c r="D22" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>5028258.59327613</v>
+        <v>4998531.5290436288</v>
       </c>
       <c r="E22" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1775043.0842606986</v>
+        <v>1765333.158302071</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
@@ -12774,11 +12774,11 @@
       </c>
       <c r="H22" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2513326.610006928</v>
+        <v>2486174.4129707455</v>
       </c>
       <c r="I22" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3455183.6645810818</v>
+        <v>3443966.4121572562</v>
       </c>
       <c r="J22" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12786,51 +12786,51 @@
       </c>
       <c r="K22" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>574785.58623469959</v>
+        <v>573321.26147515886</v>
       </c>
       <c r="L22" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>574785.58623469959</v>
+        <v>573321.26147515886</v>
       </c>
       <c r="M22" s="4">
         <f>B22*'Coal Cost Multipliers'!$B$33</f>
-        <v>4781642.2683882229</v>
+        <v>4757088.0381840812</v>
       </c>
       <c r="N22" s="4">
         <v>0</v>
       </c>
       <c r="O22" s="4">
         <f t="shared" si="0"/>
-        <v>574785.58623469959</v>
+        <v>573321.26147515886</v>
       </c>
       <c r="P22" s="4">
         <f t="shared" si="1"/>
-        <v>574785.58623469959</v>
+        <v>573321.26147515886</v>
       </c>
       <c r="Q22" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1310848.1885362437</v>
+        <v>1306592.5204017661</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B23" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4104680.723820759</v>
+        <v>4084014.7285643537</v>
       </c>
       <c r="C23" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>866070.37401335512</v>
+        <v>863860.25524858502</v>
       </c>
       <c r="D23" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4998531.5290436288</v>
+        <v>4969440.6376708252</v>
       </c>
       <c r="E23" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1765333.158302071</v>
+        <v>1755623.2323434441</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -12840,11 +12840,11 @@
       </c>
       <c r="H23" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2486174.4129707455</v>
+        <v>2459022.2159345644</v>
       </c>
       <c r="I23" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3443966.4121572562</v>
+        <v>3433160.4520611921</v>
       </c>
       <c r="J23" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12852,51 +12852,51 @@
       </c>
       <c r="K23" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>573321.26147515886</v>
+        <v>571929.01977696037</v>
       </c>
       <c r="L23" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>573321.26147515886</v>
+        <v>571929.01977696037</v>
       </c>
       <c r="M23" s="4">
         <f>B23*'Coal Cost Multipliers'!$B$33</f>
-        <v>4757088.0381840812</v>
+        <v>4733137.3425158681</v>
       </c>
       <c r="N23" s="4">
         <v>0</v>
       </c>
       <c r="O23" s="4">
         <f t="shared" si="0"/>
-        <v>573321.26147515886</v>
+        <v>571929.01977696037</v>
       </c>
       <c r="P23" s="4">
         <f t="shared" si="1"/>
-        <v>573321.26147515886</v>
+        <v>571929.01977696037</v>
       </c>
       <c r="Q23" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1306592.5204017661</v>
+        <v>1302492.8908039173</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B24" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4084014.7285643537</v>
+        <v>4067550.5033159018</v>
       </c>
       <c r="C24" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>863860.25524858502</v>
+        <v>862540.48501902213</v>
       </c>
       <c r="D24" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4969440.6376708252</v>
+        <v>4945459.5905335443</v>
       </c>
       <c r="E24" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1755623.2323434441</v>
+        <v>1745913.3063848168</v>
       </c>
       <c r="F24" s="4">
         <v>0</v>
@@ -12906,11 +12906,11 @@
       </c>
       <c r="H24" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2459022.2159345644</v>
+        <v>2431870.0188983819</v>
       </c>
       <c r="I24" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3433160.4520611921</v>
+        <v>3425700.1078922306</v>
       </c>
       <c r="J24" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12918,51 +12918,51 @@
       </c>
       <c r="K24" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>571929.01977696037</v>
+        <v>571126.25277404871</v>
       </c>
       <c r="L24" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>571929.01977696037</v>
+        <v>571126.25277404871</v>
       </c>
       <c r="M24" s="4">
         <f>B24*'Coal Cost Multipliers'!$B$33</f>
-        <v>4733137.3425158681</v>
+        <v>4714056.2557621887</v>
       </c>
       <c r="N24" s="4">
         <v>0</v>
       </c>
       <c r="O24" s="4">
         <f t="shared" si="0"/>
-        <v>571929.01977696037</v>
+        <v>571126.25277404871</v>
       </c>
       <c r="P24" s="4">
         <f t="shared" si="1"/>
-        <v>571929.01977696037</v>
+        <v>571126.25277404871</v>
       </c>
       <c r="Q24" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1302492.8908039173</v>
+        <v>1299662.5409327983</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="1">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B25" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4067550.5033159018</v>
+        <v>4041919.4833016312</v>
       </c>
       <c r="C25" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>862540.48501902213</v>
+        <v>859275.63459266303</v>
       </c>
       <c r="D25" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4945459.5905335443</v>
+        <v>4910336.3730173539</v>
       </c>
       <c r="E25" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1745913.3063848168</v>
+        <v>1736203.3804261896</v>
       </c>
       <c r="F25" s="4">
         <v>0</v>
@@ -12972,11 +12972,11 @@
       </c>
       <c r="H25" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2431870.0188983819</v>
+        <v>2404717.8218621998</v>
       </c>
       <c r="I25" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3425700.1078922306</v>
+        <v>3410933.8741836962</v>
       </c>
       <c r="J25" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -12984,51 +12984,51 @@
       </c>
       <c r="K25" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>571126.25277404871</v>
+        <v>569035.57651885482</v>
       </c>
       <c r="L25" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>571126.25277404871</v>
+        <v>569035.57651885482</v>
       </c>
       <c r="M25" s="4">
         <f>B25*'Coal Cost Multipliers'!$B$33</f>
-        <v>4714056.2557621887</v>
+        <v>4684351.3829790875</v>
       </c>
       <c r="N25" s="4">
         <v>0</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>571126.25277404871</v>
+        <v>569035.57651885482</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="1"/>
-        <v>571126.25277404871</v>
+        <v>569035.57651885482</v>
       </c>
       <c r="Q25" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1299662.5409327983</v>
+        <v>1294060.4391091652</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="1">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B26" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4041919.4833016312</v>
+        <v>4027549.0846800846</v>
       </c>
       <c r="C26" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>859275.63459266303</v>
+        <v>858404.68064265454</v>
       </c>
       <c r="D26" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4910336.3730173539</v>
+        <v>4888892.5746857012</v>
       </c>
       <c r="E26" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1736203.3804261896</v>
+        <v>1726493.454467562</v>
       </c>
       <c r="F26" s="4">
         <v>0</v>
@@ -13038,11 +13038,11 @@
       </c>
       <c r="H26" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2404717.8218621998</v>
+        <v>2377565.6248260182</v>
       </c>
       <c r="I26" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3410933.8741836962</v>
+        <v>3405154.6476856545</v>
       </c>
       <c r="J26" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -13050,51 +13050,51 @@
       </c>
       <c r="K26" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>569035.57651885482</v>
+        <v>568530.177953306</v>
       </c>
       <c r="L26" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>569035.57651885482</v>
+        <v>568530.177953306</v>
       </c>
       <c r="M26" s="4">
         <f>B26*'Coal Cost Multipliers'!$B$33</f>
-        <v>4684351.3829790875</v>
+        <v>4667696.920431057</v>
       </c>
       <c r="N26" s="4">
         <v>0</v>
       </c>
       <c r="O26" s="4">
         <f t="shared" si="0"/>
-        <v>569035.57651885482</v>
+        <v>568530.177953306</v>
       </c>
       <c r="P26" s="4">
         <f t="shared" si="1"/>
-        <v>569035.57651885482</v>
+        <v>568530.177953306</v>
       </c>
       <c r="Q26" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1294060.4391091652</v>
+        <v>1291867.8816877592</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B27" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4027549.0846800846</v>
+        <v>4002808.235279711</v>
       </c>
       <c r="C27" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>858404.68064265454</v>
+        <v>855323.90187924227</v>
       </c>
       <c r="D27" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4888892.5746857012</v>
+        <v>4854859.1300343601</v>
       </c>
       <c r="E27" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1726493.454467562</v>
+        <v>1716783.5285089349</v>
       </c>
       <c r="F27" s="4">
         <v>0</v>
@@ -13104,11 +13104,11 @@
       </c>
       <c r="H27" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2377565.6248260182</v>
+        <v>2350413.4277898367</v>
       </c>
       <c r="I27" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3405154.6476856545</v>
+        <v>3391084.6066551027</v>
       </c>
       <c r="J27" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -13116,51 +13116,51 @@
       </c>
       <c r="K27" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>568530.177953306</v>
+        <v>566561.19400174171</v>
       </c>
       <c r="L27" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>568530.177953306</v>
+        <v>566561.19400174171</v>
       </c>
       <c r="M27" s="4">
         <f>B27*'Coal Cost Multipliers'!$B$33</f>
-        <v>4667696.920431057</v>
+        <v>4639023.7040091278</v>
       </c>
       <c r="N27" s="4">
         <v>0</v>
       </c>
       <c r="O27" s="4">
         <f t="shared" si="0"/>
-        <v>568530.177953306</v>
+        <v>566561.19400174171</v>
       </c>
       <c r="P27" s="4">
         <f t="shared" si="1"/>
-        <v>568530.177953306</v>
+        <v>566561.19400174171</v>
       </c>
       <c r="Q27" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1291867.8816877592</v>
+        <v>1286529.9055950278</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="1">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B28" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>4002808.235279711</v>
+        <v>3987525.789950409</v>
       </c>
       <c r="C28" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>855323.90187924227</v>
+        <v>854264.07546210196</v>
       </c>
       <c r="D28" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4854859.1300343601</v>
+        <v>4832297.6878896719</v>
       </c>
       <c r="E28" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1716783.5285089349</v>
+        <v>1707073.6025503075</v>
       </c>
       <c r="F28" s="4">
         <v>0</v>
@@ -13170,11 +13170,11 @@
       </c>
       <c r="H28" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2350413.4277898367</v>
+        <v>2323261.2307536541</v>
       </c>
       <c r="I28" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3391084.6066551027</v>
+        <v>3384590.2237373139</v>
       </c>
       <c r="J28" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -13182,51 +13182,51 @@
       </c>
       <c r="K28" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>566561.19400174171</v>
+        <v>565930.83880835248</v>
       </c>
       <c r="L28" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>566561.19400174171</v>
+        <v>565930.83880835248</v>
       </c>
       <c r="M28" s="4">
         <f>B28*'Coal Cost Multipliers'!$B$33</f>
-        <v>4639023.7040091278</v>
+        <v>4621312.2319698231</v>
       </c>
       <c r="N28" s="4">
         <v>0</v>
       </c>
       <c r="O28" s="4">
         <f t="shared" si="0"/>
-        <v>566561.19400174171</v>
+        <v>565930.83880835248</v>
       </c>
       <c r="P28" s="4">
         <f t="shared" si="1"/>
-        <v>566561.19400174171</v>
+        <v>565930.83880835248</v>
       </c>
       <c r="Q28" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1286529.9055950278</v>
+        <v>1284066.0278652529</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="1">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B29" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>3987525.789950409</v>
+        <v>3964365.0723133213</v>
       </c>
       <c r="C29" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>854264.07546210196</v>
+        <v>851517.47797442612</v>
       </c>
       <c r="D29" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4832297.6878896719</v>
+        <v>4800188.8840519451</v>
       </c>
       <c r="E29" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1707073.6025503075</v>
+        <v>1697363.6765916804</v>
       </c>
       <c r="F29" s="4">
         <v>0</v>
@@ -13236,11 +13236,11 @@
       </c>
       <c r="H29" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2323261.2307536541</v>
+        <v>2296109.0337174726</v>
       </c>
       <c r="I29" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3384590.2237373139</v>
+        <v>3371777.3022148283</v>
       </c>
       <c r="J29" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -13248,51 +13248,51 @@
       </c>
       <c r="K29" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>565930.83880835248</v>
+        <v>564183.11255323095</v>
       </c>
       <c r="L29" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>565930.83880835248</v>
+        <v>564183.11255323095</v>
       </c>
       <c r="M29" s="4">
         <f>B29*'Coal Cost Multipliers'!$B$33</f>
-        <v>4621312.2319698231</v>
+        <v>4594470.2970568947</v>
       </c>
       <c r="N29" s="4">
         <v>0</v>
       </c>
       <c r="O29" s="4">
         <f t="shared" si="0"/>
-        <v>565930.83880835248</v>
+        <v>564183.11255323095</v>
       </c>
       <c r="P29" s="4">
         <f t="shared" si="1"/>
-        <v>565930.83880835248</v>
+        <v>564183.11255323095</v>
       </c>
       <c r="Q29" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1284066.0278652529</v>
+        <v>1279204.9852700992</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="1">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B30" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>3964365.0723133213</v>
+        <v>3944904.6700286916</v>
       </c>
       <c r="C30" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>851517.47797442612</v>
+        <v>849564.13218949281</v>
       </c>
       <c r="D30" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4800188.8840519451</v>
+        <v>4772563.1483514039</v>
       </c>
       <c r="E30" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1697363.6765916804</v>
+        <v>1687653.7506330532</v>
       </c>
       <c r="F30" s="4">
         <v>0</v>
@@ -13302,11 +13302,11 @@
       </c>
       <c r="H30" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2296109.0337174726</v>
+        <v>2268956.8366812905</v>
       </c>
       <c r="I30" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3371777.3022148283</v>
+        <v>3361934.7756505935</v>
       </c>
       <c r="J30" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -13314,51 +13314,51 @@
       </c>
       <c r="K30" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>564183.11255323095</v>
+        <v>562960.8983085549</v>
       </c>
       <c r="L30" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>564183.11255323095</v>
+        <v>562960.8983085549</v>
       </c>
       <c r="M30" s="4">
         <f>B30*'Coal Cost Multipliers'!$B$33</f>
-        <v>4594470.2970568947</v>
+        <v>4571916.8140565678</v>
       </c>
       <c r="N30" s="4">
         <v>0</v>
       </c>
       <c r="O30" s="4">
         <f t="shared" si="0"/>
-        <v>564183.11255323095</v>
+        <v>562960.8983085549</v>
       </c>
       <c r="P30" s="4">
         <f t="shared" si="1"/>
-        <v>564183.11255323095</v>
+        <v>562960.8983085549</v>
       </c>
       <c r="Q30" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1279204.9852700992</v>
+        <v>1275470.8688323523</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="1">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B31" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>3944904.6700286916</v>
+        <v>3925379.2073251978</v>
       </c>
       <c r="C31" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>849564.13218949281</v>
+        <v>847597.09481380892</v>
       </c>
       <c r="D31" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4772563.1483514039</v>
+        <v>4744855.6043133195</v>
       </c>
       <c r="E31" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1687653.7506330532</v>
+        <v>1677943.8246744261</v>
       </c>
       <c r="F31" s="4">
         <v>0</v>
@@ -13368,11 +13368,11 @@
       </c>
       <c r="H31" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2268956.8366812905</v>
+        <v>2241804.6396451085</v>
       </c>
       <c r="I31" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3361934.7756505935</v>
+        <v>3352040.6597777726</v>
       </c>
       <c r="J31" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -13380,51 +13380,51 @@
       </c>
       <c r="K31" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>562960.8983085549</v>
+        <v>561729.66530371504</v>
       </c>
       <c r="L31" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>562960.8983085549</v>
+        <v>561729.66530371504</v>
       </c>
       <c r="M31" s="4">
         <f>B31*'Coal Cost Multipliers'!$B$33</f>
-        <v>4571916.8140565678</v>
+        <v>4549287.9297860414</v>
       </c>
       <c r="N31" s="4">
         <v>0</v>
       </c>
       <c r="O31" s="4">
         <f t="shared" si="0"/>
-        <v>562960.8983085549</v>
+        <v>561729.66530371504</v>
       </c>
       <c r="P31" s="4">
         <f t="shared" si="1"/>
-        <v>562960.8983085549</v>
+        <v>561729.66530371504</v>
       </c>
       <c r="Q31" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1275470.8688323523</v>
+        <v>1271717.1801349882</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="1">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B32" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>3925379.2073251978</v>
+        <v>3905501.7363179387</v>
       </c>
       <c r="C32" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>847597.09481380892</v>
+        <v>845554.54963951895</v>
       </c>
       <c r="D32" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4744855.6043133195</v>
+        <v>4716723.1390827727</v>
       </c>
       <c r="E32" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1677943.8246744261</v>
+        <v>1668233.898715799</v>
       </c>
       <c r="F32" s="4">
         <v>0</v>
@@ -13434,11 +13434,11 @@
       </c>
       <c r="H32" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2241804.6396451085</v>
+        <v>2214652.4426089264</v>
       </c>
       <c r="I32" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3352040.6597777726</v>
+        <v>3341863.5705453139</v>
       </c>
       <c r="J32" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -13446,51 +13446,51 @@
       </c>
       <c r="K32" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>561729.66530371504</v>
+        <v>560448.29901305423</v>
       </c>
       <c r="L32" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>561729.66530371504</v>
+        <v>560448.29901305423</v>
       </c>
       <c r="M32" s="4">
         <f>B32*'Coal Cost Multipliers'!$B$33</f>
-        <v>4549287.9297860414</v>
+        <v>4526251.0882092463</v>
       </c>
       <c r="N32" s="4">
         <v>0</v>
       </c>
       <c r="O32" s="4">
         <f t="shared" si="0"/>
-        <v>561729.66530371504</v>
+        <v>560448.29901305423</v>
       </c>
       <c r="P32" s="4">
         <f t="shared" si="1"/>
-        <v>561729.66530371504</v>
+        <v>560448.29901305423</v>
       </c>
       <c r="Q32" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1271717.1801349882</v>
+        <v>1267856.1353165335</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="1">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B33" s="4">
         <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>3905501.7363179387</v>
+        <v>3855675.0986996656</v>
       </c>
       <c r="C33" s="4">
         <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>845554.54963951895</v>
+        <v>837010.54636717902</v>
       </c>
       <c r="D33" s="4">
         <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4716723.1390827727</v>
+        <v>4652452.4766705297</v>
       </c>
       <c r="E33" s="4">
         <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1668233.898715799</v>
+        <v>1658523.9727571718</v>
       </c>
       <c r="F33" s="4">
         <v>0</v>
@@ -13500,11 +13500,11 @@
       </c>
       <c r="H33" s="4">
         <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2214652.4426089264</v>
+        <v>2187500.2455727453</v>
       </c>
       <c r="I33" s="4">
         <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3341863.5705453139</v>
+        <v>3307435.7945322236</v>
       </c>
       <c r="J33" s="4">
         <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
@@ -13512,97 +13512,34 @@
       </c>
       <c r="K33" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>560448.29901305423</v>
+        <v>554857.17842271458</v>
       </c>
       <c r="L33" s="4">
         <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>560448.29901305423</v>
+        <v>554857.17842271458</v>
       </c>
       <c r="M33" s="4">
         <f>B33*'Coal Cost Multipliers'!$B$33</f>
-        <v>4526251.0882092463</v>
+        <v>4468504.8911856236</v>
       </c>
       <c r="N33" s="4">
         <v>0</v>
       </c>
       <c r="O33" s="4">
         <f t="shared" si="0"/>
-        <v>560448.29901305423</v>
+        <v>554857.17842271458</v>
       </c>
       <c r="P33" s="4">
         <f t="shared" si="1"/>
-        <v>560448.29901305423</v>
+        <v>554857.17842271458</v>
       </c>
       <c r="Q33" s="4">
         <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1267856.1353165335</v>
+        <v>1254794.7202940234</v>
       </c>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="1">
-        <v>2050</v>
-      </c>
-      <c r="B34" s="4">
-        <f>'EIA Costs'!$D$3*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("coal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$69</f>
-        <v>3855675.0986996656</v>
-      </c>
-      <c r="C34" s="4">
-        <f>'EIA Costs'!$D$5*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas nonpeaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>837010.54636717902</v>
-      </c>
-      <c r="D34" s="4">
-        <f>'EIA Costs'!$D$8*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("nuclear",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>4652452.4766705297</v>
-      </c>
-      <c r="E34" s="4">
-        <f>'EIA Costs'!$D$11*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("hydro",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1658523.9727571718</v>
-      </c>
-      <c r="F34" s="4">
-        <v>0</v>
-      </c>
-      <c r="G34" s="4">
-        <v>0</v>
-      </c>
-      <c r="H34" s="4">
-        <f>'EIA Costs'!$D$14*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("solar thermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>2187500.2455727453</v>
-      </c>
-      <c r="I34" s="4">
-        <f>'EIA Costs'!$D$9*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>3307435.7945322236</v>
-      </c>
-      <c r="J34" s="4">
-        <f>'EIA Costs'!$D$10*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("geothermal",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>640953.95192689588</v>
-      </c>
-      <c r="K34" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>554857.17842271458</v>
-      </c>
-      <c r="L34" s="4">
-        <f>'EIA Costs'!$D$7*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("natural gas peaker",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>554857.17842271458</v>
-      </c>
-      <c r="M34" s="4">
-        <f>B34*'Coal Cost Multipliers'!$B$33</f>
-        <v>4468504.8911856236</v>
-      </c>
-      <c r="N34" s="4">
-        <v>0</v>
-      </c>
-      <c r="O34" s="4">
-        <f t="shared" si="0"/>
-        <v>554857.17842271458</v>
-      </c>
-      <c r="P34" s="4">
-        <f t="shared" si="1"/>
-        <v>554857.17842271458</v>
-      </c>
-      <c r="Q34" s="4">
-        <f>'EIA Costs'!$D$16*INDEX('Cost Improvement and Off Wnd'!$B$63:$AI$71,MATCH("biomass",'Cost Improvement and Off Wnd'!$A$63:$A$71,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement and Off Wnd'!$B$62:$AI$62,0))*1000*About!$A$73</f>
-        <v>1254794.7202940234</v>
-      </c>
+      <c r="B34" s="12"/>
     </row>
     <row r="35" spans="1:17">
       <c r="B35" s="12"/>
@@ -13639,9 +13576,6 @@
     </row>
     <row r="46" spans="1:17">
       <c r="B46" s="12"/>
-    </row>
-    <row r="47" spans="1:17">
-      <c r="B47" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>